<commit_message>
update returns data (Sep 2021)
</commit_message>
<xml_diff>
--- a/EquityHedging/data/update_strats/put_spread_data.xlsx
+++ b/EquityHedging/data/update_strats/put_spread_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pforj\Documents\ups\RMP\EquityHedging\data\update_strats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34B1C64-D9F5-453C-8BBD-1EA88402B92D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7EE51D9A-A518-4E59-B8FE-12FDE2955B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
     <definedName name="solver_typ" hidden="1">3</definedName>
     <definedName name="solver_val" hidden="1">0</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Put Spread</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>Disclaimer</t>
-  </si>
-  <si>
-    <t>August 31, 2021</t>
   </si>
 </sst>
 </file>
@@ -225,10 +222,10 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1015,13 +1012,12 @@
   </sheetPr>
   <dimension ref="B9:B25"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="9" spans="2:2" ht="80.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1045,8 +1041,8 @@
       </c>
     </row>
     <row r="21" spans="2:2" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B21" s="21" t="s">
-        <v>10</v>
+      <c r="B21" s="22">
+        <v>44469</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
@@ -1076,11 +1072,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D191"/>
+  <dimension ref="A1:D192"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A190" sqref="A190"/>
+      <pane ySplit="2" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A192" sqref="A192:D192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3755,6 +3751,20 @@
         <v>-1.4380003728869939E-3</v>
       </c>
     </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192" s="1">
+        <v>44469</v>
+      </c>
+      <c r="B192" s="12">
+        <v>2.3749385267922918E-2</v>
+      </c>
+      <c r="C192" s="12">
+        <v>-5.1286337737017629E-3</v>
+      </c>
+      <c r="D192" s="12">
+        <v>1.8620751494221155E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3762,11 +3772,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D3923"/>
+  <dimension ref="A1:D3944"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3890" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3924" sqref="B3924"/>
+      <pane ySplit="2" topLeftCell="A3920" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3944" sqref="A3944"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58087,13 +58097,13 @@
       <c r="A3881" s="1">
         <v>44378</v>
       </c>
-      <c r="B3881" s="22">
+      <c r="B3881" s="21">
         <v>-1.6149636355186302E-3</v>
       </c>
-      <c r="C3881" s="22">
+      <c r="C3881" s="21">
         <v>3.5785425016731162E-4</v>
       </c>
-      <c r="D3881" s="22">
+      <c r="D3881" s="21">
         <v>-1.2571093853513185E-3</v>
       </c>
     </row>
@@ -58101,13 +58111,13 @@
       <c r="A3882" s="1">
         <v>44379</v>
       </c>
-      <c r="B3882" s="22">
+      <c r="B3882" s="21">
         <v>-2.1842529418430261E-3</v>
       </c>
-      <c r="C3882" s="22">
+      <c r="C3882" s="21">
         <v>4.9818269124531902E-4</v>
       </c>
-      <c r="D3882" s="22">
+      <c r="D3882" s="21">
         <v>-1.6860702505977071E-3</v>
       </c>
     </row>
@@ -58115,13 +58125,13 @@
       <c r="A3883" s="1">
         <v>44383</v>
       </c>
-      <c r="B3883" s="22">
+      <c r="B3883" s="21">
         <v>5.3575955116370877E-4</v>
       </c>
-      <c r="C3883" s="22">
+      <c r="C3883" s="21">
         <v>-1.9030467684140142E-4</v>
       </c>
-      <c r="D3883" s="22">
+      <c r="D3883" s="21">
         <v>3.4545487432230735E-4</v>
       </c>
     </row>
@@ -58129,13 +58139,13 @@
       <c r="A3884" s="1">
         <v>44384</v>
       </c>
-      <c r="B3884" s="22">
+      <c r="B3884" s="21">
         <v>-9.9690696764109603E-4</v>
       </c>
-      <c r="C3884" s="22">
+      <c r="C3884" s="21">
         <v>2.8566969818103318E-4</v>
       </c>
-      <c r="D3884" s="22">
+      <c r="D3884" s="21">
         <v>-7.1123726946006286E-4</v>
       </c>
     </row>
@@ -58143,13 +58153,13 @@
       <c r="A3885" s="1">
         <v>44385</v>
       </c>
-      <c r="B3885" s="22">
+      <c r="B3885" s="21">
         <v>2.1714204308047416E-3</v>
       </c>
-      <c r="C3885" s="22">
+      <c r="C3885" s="21">
         <v>-1.2918810542449535E-3</v>
       </c>
-      <c r="D3885" s="22">
+      <c r="D3885" s="21">
         <v>8.7953937655978805E-4</v>
       </c>
     </row>
@@ -58157,13 +58167,13 @@
       <c r="A3886" s="1">
         <v>44386</v>
       </c>
-      <c r="B3886" s="22">
+      <c r="B3886" s="21">
         <v>-3.3325277202208765E-3</v>
       </c>
-      <c r="C3886" s="22">
+      <c r="C3886" s="21">
         <v>1.5277295925271786E-3</v>
       </c>
-      <c r="D3886" s="22">
+      <c r="D3886" s="21">
         <v>-1.8047981276936979E-3</v>
       </c>
     </row>
@@ -58171,13 +58181,13 @@
       <c r="A3887" s="1">
         <v>44389</v>
       </c>
-      <c r="B3887" s="22">
+      <c r="B3887" s="21">
         <v>-9.3182929799353025E-4</v>
       </c>
-      <c r="C3887" s="22">
+      <c r="C3887" s="21">
         <v>4.1540924896370089E-4</v>
       </c>
-      <c r="D3887" s="22">
+      <c r="D3887" s="21">
         <v>-5.1642004902982932E-4</v>
       </c>
     </row>
@@ -58185,13 +58195,13 @@
       <c r="A3888" s="1">
         <v>44390</v>
       </c>
-      <c r="B3888" s="22">
+      <c r="B3888" s="21">
         <v>7.9320836168593391E-4</v>
       </c>
-      <c r="C3888" s="22">
+      <c r="C3888" s="21">
         <v>-3.4040711733421226E-4</v>
       </c>
-      <c r="D3888" s="22">
+      <c r="D3888" s="21">
         <v>4.5280124435172165E-4</v>
       </c>
     </row>
@@ -58199,13 +58209,13 @@
       <c r="A3889" s="1">
         <v>44391</v>
       </c>
-      <c r="B3889" s="22">
+      <c r="B3889" s="21">
         <v>-3.6763410713256805E-4</v>
       </c>
-      <c r="C3889" s="22">
+      <c r="C3889" s="21">
         <v>4.2585416020906111E-4</v>
       </c>
-      <c r="D3889" s="22">
+      <c r="D3889" s="21">
         <v>5.8220053076493065E-5</v>
       </c>
     </row>
@@ -58213,13 +58223,13 @@
       <c r="A3890" s="1">
         <v>44392</v>
       </c>
-      <c r="B3890" s="22">
+      <c r="B3890" s="21">
         <v>8.450697045676714E-4</v>
       </c>
-      <c r="C3890" s="22">
+      <c r="C3890" s="21">
         <v>-2.4625715863417605E-4</v>
       </c>
-      <c r="D3890" s="22">
+      <c r="D3890" s="21">
         <v>5.9881254593349535E-4</v>
       </c>
     </row>
@@ -58227,13 +58237,13 @@
       <c r="A3891" s="1">
         <v>44393</v>
       </c>
-      <c r="B3891" s="22">
+      <c r="B3891" s="21">
         <v>1.9475350422432287E-3</v>
       </c>
-      <c r="C3891" s="22">
+      <c r="C3891" s="21">
         <v>-6.623618272589446E-4</v>
       </c>
-      <c r="D3891" s="22">
+      <c r="D3891" s="21">
         <v>1.285173214984284E-3</v>
       </c>
     </row>
@@ -58241,13 +58251,13 @@
       <c r="A3892" s="1">
         <v>44396</v>
       </c>
-      <c r="B3892" s="22">
+      <c r="B3892" s="21">
         <v>4.5471354732311686E-3</v>
       </c>
-      <c r="C3892" s="22">
+      <c r="C3892" s="21">
         <v>-1.9311988781355264E-3</v>
       </c>
-      <c r="D3892" s="22">
+      <c r="D3892" s="21">
         <v>2.6159365950956422E-3</v>
       </c>
     </row>
@@ -58255,13 +58265,13 @@
       <c r="A3893" s="1">
         <v>44397</v>
       </c>
-      <c r="B3893" s="22">
+      <c r="B3893" s="21">
         <v>-5.5136682132533614E-3</v>
       </c>
-      <c r="C3893" s="22">
+      <c r="C3893" s="21">
         <v>1.8993633073112778E-3</v>
       </c>
-      <c r="D3893" s="22">
+      <c r="D3893" s="21">
         <v>-3.6143049059420835E-3</v>
       </c>
     </row>
@@ -58269,13 +58279,13 @@
       <c r="A3894" s="1">
         <v>44398</v>
       </c>
-      <c r="B3894" s="22">
+      <c r="B3894" s="21">
         <v>-2.3125398005522011E-3</v>
       </c>
-      <c r="C3894" s="22">
+      <c r="C3894" s="21">
         <v>1.0176600274760621E-3</v>
       </c>
-      <c r="D3894" s="22">
+      <c r="D3894" s="21">
         <v>-1.294879773076139E-3</v>
       </c>
     </row>
@@ -58283,13 +58293,13 @@
       <c r="A3895" s="1">
         <v>44399</v>
       </c>
-      <c r="B3895" s="22">
+      <c r="B3895" s="21">
         <v>-5.0290484865755665E-4</v>
       </c>
-      <c r="C3895" s="22">
+      <c r="C3895" s="21">
         <v>1.7933479947460562E-4</v>
       </c>
-      <c r="D3895" s="22">
+      <c r="D3895" s="21">
         <v>-3.2357004918295103E-4</v>
       </c>
     </row>
@@ -58297,13 +58307,13 @@
       <c r="A3896" s="1">
         <v>44400</v>
       </c>
-      <c r="B3896" s="22">
+      <c r="B3896" s="21">
         <v>-2.3242483280770348E-3</v>
       </c>
-      <c r="C3896" s="22">
+      <c r="C3896" s="21">
         <v>4.1920262460881668E-4</v>
       </c>
-      <c r="D3896" s="22">
+      <c r="D3896" s="21">
         <v>-1.9050457034682181E-3</v>
       </c>
     </row>
@@ -58311,13 +58321,13 @@
       <c r="A3897" s="1">
         <v>44403</v>
       </c>
-      <c r="B3897" s="22">
+      <c r="B3897" s="21">
         <v>-4.9717213013058842E-4</v>
       </c>
-      <c r="C3897" s="22">
+      <c r="C3897" s="21">
         <v>3.9190691857141064E-4</v>
       </c>
-      <c r="D3897" s="22">
+      <c r="D3897" s="21">
         <v>-1.0526521155917779E-4</v>
       </c>
     </row>
@@ -58325,13 +58335,13 @@
       <c r="A3898" s="1">
         <v>44404</v>
       </c>
-      <c r="B3898" s="22">
+      <c r="B3898" s="21">
         <v>7.9926512031273066E-4</v>
       </c>
-      <c r="C3898" s="22">
+      <c r="C3898" s="21">
         <v>-5.1726547128750884E-4</v>
       </c>
-      <c r="D3898" s="22">
+      <c r="D3898" s="21">
         <v>2.8199964902522181E-4</v>
       </c>
     </row>
@@ -58339,13 +58349,13 @@
       <c r="A3899" s="1">
         <v>44405</v>
       </c>
-      <c r="B3899" s="22">
+      <c r="B3899" s="21">
         <v>3.8697045324472425E-5</v>
       </c>
-      <c r="C3899" s="22">
+      <c r="C3899" s="21">
         <v>4.5813632143458521E-4</v>
       </c>
-      <c r="D3899" s="22">
+      <c r="D3899" s="21">
         <v>4.968333667590576E-4</v>
       </c>
     </row>
@@ -58353,13 +58363,13 @@
       <c r="A3900" s="1">
         <v>44406</v>
       </c>
-      <c r="B3900" s="22">
+      <c r="B3900" s="21">
         <v>-8.0040052365767174E-4</v>
       </c>
-      <c r="C3900" s="22">
+      <c r="C3900" s="21">
         <v>2.7256262214815711E-4</v>
       </c>
-      <c r="D3900" s="22">
+      <c r="D3900" s="21">
         <v>-5.2783790150951458E-4</v>
       </c>
     </row>
@@ -58367,13 +58377,13 @@
       <c r="A3901" s="1">
         <v>44407</v>
       </c>
-      <c r="B3901" s="22">
+      <c r="B3901" s="21">
         <v>8.8609413809032046E-4</v>
       </c>
-      <c r="C3901" s="22">
+      <c r="C3901" s="21">
         <v>-1.4304295231616754E-4</v>
       </c>
-      <c r="D3901" s="22">
+      <c r="D3901" s="21">
         <v>7.4305118577415289E-4</v>
       </c>
     </row>
@@ -58381,13 +58391,13 @@
       <c r="A3902" s="1">
         <v>44410</v>
       </c>
-      <c r="B3902" s="22">
+      <c r="B3902" s="21">
         <v>4.1013577723438585E-4</v>
       </c>
-      <c r="C3902" s="22">
+      <c r="C3902" s="21">
         <v>1.4247339631872252E-5</v>
       </c>
-      <c r="D3902" s="22">
+      <c r="D3902" s="21">
         <v>4.2438311686625812E-4</v>
       </c>
     </row>
@@ -58395,13 +58405,13 @@
       <c r="A3903" s="1">
         <v>44411</v>
       </c>
-      <c r="B3903" s="22">
+      <c r="B3903" s="21">
         <v>-1.5485713786333925E-3</v>
       </c>
-      <c r="C3903" s="22">
+      <c r="C3903" s="21">
         <v>4.6052193175976931E-4</v>
       </c>
-      <c r="D3903" s="22">
+      <c r="D3903" s="21">
         <v>-1.0880494468736232E-3</v>
       </c>
     </row>
@@ -58409,13 +58419,13 @@
       <c r="A3904" s="1">
         <v>44412</v>
       </c>
-      <c r="B3904" s="22">
+      <c r="B3904" s="21">
         <v>7.3105981950567897E-4</v>
       </c>
-      <c r="C3904" s="22">
+      <c r="C3904" s="21">
         <v>9.6089300804043967E-5</v>
       </c>
-      <c r="D3904" s="22">
+      <c r="D3904" s="21">
         <v>8.2714912030972291E-4</v>
       </c>
     </row>
@@ -58423,13 +58433,13 @@
       <c r="A3905" s="1">
         <v>44413</v>
       </c>
-      <c r="B3905" s="22">
+      <c r="B3905" s="21">
         <v>-9.8590317767043674E-4</v>
       </c>
-      <c r="C3905" s="22">
+      <c r="C3905" s="21">
         <v>2.2281264863377949E-4</v>
       </c>
-      <c r="D3905" s="22">
+      <c r="D3905" s="21">
         <v>-7.6309052903665727E-4</v>
       </c>
     </row>
@@ -58437,13 +58447,13 @@
       <c r="A3906" s="1">
         <v>44414</v>
       </c>
-      <c r="B3906" s="22">
+      <c r="B3906" s="21">
         <v>-2.3966106328389715E-4</v>
       </c>
-      <c r="C3906" s="22">
+      <c r="C3906" s="21">
         <v>2.5567156279150948E-4</v>
       </c>
-      <c r="D3906" s="22">
+      <c r="D3906" s="21">
         <v>1.6010499507612333E-5</v>
       </c>
     </row>
@@ -58451,13 +58461,13 @@
       <c r="A3907" s="1">
         <v>44417</v>
       </c>
-      <c r="B3907" s="22">
+      <c r="B3907" s="21">
         <v>9.5657228547675423E-5</v>
       </c>
-      <c r="C3907" s="22">
+      <c r="C3907" s="21">
         <v>8.2333964077408847E-5</v>
       </c>
-      <c r="D3907" s="22">
+      <c r="D3907" s="21">
         <v>1.7799119262508427E-4</v>
       </c>
     </row>
@@ -58465,13 +58475,13 @@
       <c r="A3908" s="1">
         <v>44418</v>
       </c>
-      <c r="B3908" s="22">
+      <c r="B3908" s="21">
         <v>-1.0566205177843369E-4</v>
       </c>
-      <c r="C3908" s="22">
+      <c r="C3908" s="21">
         <v>1.1568064091808075E-5</v>
       </c>
-      <c r="D3908" s="22">
+      <c r="D3908" s="21">
         <v>-9.409398768662561E-5</v>
       </c>
     </row>
@@ -58479,13 +58489,13 @@
       <c r="A3909" s="1">
         <v>44419</v>
       </c>
-      <c r="B3909" s="22">
+      <c r="B3909" s="21">
         <v>-2.6342637227794478E-4</v>
       </c>
-      <c r="C3909" s="22">
+      <c r="C3909" s="21">
         <v>1.6010934922942031E-4</v>
       </c>
-      <c r="D3909" s="22">
+      <c r="D3909" s="21">
         <v>-1.0331702304852447E-4</v>
       </c>
     </row>
@@ -58493,13 +58503,13 @@
       <c r="A3910" s="1">
         <v>44420</v>
       </c>
-      <c r="B3910" s="22">
+      <c r="B3910" s="21">
         <v>-2.8224180552861107E-4</v>
       </c>
-      <c r="C3910" s="22">
+      <c r="C3910" s="21">
         <v>8.4125451923803567E-5</v>
       </c>
-      <c r="D3910" s="22">
+      <c r="D3910" s="21">
         <v>-1.9811635360480752E-4</v>
       </c>
     </row>
@@ -58507,13 +58517,13 @@
       <c r="A3911" s="1">
         <v>44421</v>
       </c>
-      <c r="B3911" s="22">
+      <c r="B3911" s="21">
         <v>-1.2865849507447444E-4</v>
       </c>
-      <c r="C3911" s="22">
+      <c r="C3911" s="21">
         <v>-2.9480776508940968E-5</v>
       </c>
-      <c r="D3911" s="22">
+      <c r="D3911" s="21">
         <v>-1.5813927158341541E-4</v>
       </c>
     </row>
@@ -58521,13 +58531,13 @@
       <c r="A3912" s="1">
         <v>44424</v>
       </c>
-      <c r="B3912" s="22">
+      <c r="B3912" s="21">
         <v>-1.6309540607083541E-4</v>
       </c>
-      <c r="C3912" s="22">
+      <c r="C3912" s="21">
         <v>5.7843944698607842E-5</v>
       </c>
-      <c r="D3912" s="22">
+      <c r="D3912" s="21">
         <v>-1.0525146137222757E-4</v>
       </c>
     </row>
@@ -58535,13 +58545,13 @@
       <c r="A3913" s="1">
         <v>44425</v>
       </c>
-      <c r="B3913" s="22">
+      <c r="B3913" s="21">
         <v>3.7178943904030842E-4</v>
       </c>
-      <c r="C3913" s="22">
+      <c r="C3913" s="21">
         <v>-1.0556606214848708E-4</v>
       </c>
-      <c r="D3913" s="22">
+      <c r="D3913" s="21">
         <v>2.6622337689182136E-4</v>
       </c>
     </row>
@@ -58549,13 +58559,13 @@
       <c r="A3914" s="1">
         <v>44426</v>
       </c>
-      <c r="B3914" s="22">
+      <c r="B3914" s="21">
         <v>8.9816330682561797E-4</v>
       </c>
-      <c r="C3914" s="22">
+      <c r="C3914" s="21">
         <v>-5.2150898665097496E-4</v>
       </c>
-      <c r="D3914" s="22">
+      <c r="D3914" s="21">
         <v>3.7665432017464301E-4</v>
       </c>
     </row>
@@ -58563,13 +58573,13 @@
       <c r="A3915" s="1">
         <v>44427</v>
       </c>
-      <c r="B3915" s="22">
+      <c r="B3915" s="21">
         <v>-2.1821992833287085E-4</v>
       </c>
-      <c r="C3915" s="22">
+      <c r="C3915" s="21">
         <v>2.2801207460511577E-4</v>
       </c>
-      <c r="D3915" s="22">
+      <c r="D3915" s="21">
         <v>9.792146272244917E-6</v>
       </c>
     </row>
@@ -58577,13 +58587,13 @@
       <c r="A3916" s="1">
         <v>44428</v>
       </c>
-      <c r="B3916" s="22">
+      <c r="B3916" s="21">
         <v>-9.6159736978749285E-4</v>
       </c>
-      <c r="C3916" s="22">
+      <c r="C3916" s="21">
         <v>4.8210665319668304E-4</v>
       </c>
-      <c r="D3916" s="22">
+      <c r="D3916" s="21">
         <v>-4.7949071659080981E-4</v>
       </c>
     </row>
@@ -58591,13 +58601,13 @@
       <c r="A3917" s="1">
         <v>44431</v>
       </c>
-      <c r="B3917" s="22">
+      <c r="B3917" s="21">
         <v>-4.8357331559152053E-4</v>
       </c>
-      <c r="C3917" s="22">
+      <c r="C3917" s="21">
         <v>9.1010398937731317E-5</v>
       </c>
-      <c r="D3917" s="22">
+      <c r="D3917" s="21">
         <v>-3.9256291665378922E-4</v>
       </c>
     </row>
@@ -58605,13 +58615,13 @@
       <c r="A3918" s="1">
         <v>44432</v>
       </c>
-      <c r="B3918" s="22">
+      <c r="B3918" s="21">
         <v>-4.0514479584468823E-5</v>
       </c>
-      <c r="C3918" s="22">
+      <c r="C3918" s="21">
         <v>3.3241598504287209E-5</v>
       </c>
-      <c r="D3918" s="22">
+      <c r="D3918" s="21">
         <v>-7.2728810801816134E-6</v>
       </c>
     </row>
@@ -58619,13 +58629,13 @@
       <c r="A3919" s="1">
         <v>44433</v>
       </c>
-      <c r="B3919" s="22">
+      <c r="B3919" s="21">
         <v>-4.9231726349268157E-5</v>
       </c>
-      <c r="C3919" s="22">
+      <c r="C3919" s="21">
         <v>3.562119458347433E-5</v>
       </c>
-      <c r="D3919" s="22">
+      <c r="D3919" s="21">
         <v>-1.3610531765793827E-5</v>
       </c>
     </row>
@@ -58633,13 +58643,13 @@
       <c r="A3920" s="1">
         <v>44434</v>
       </c>
-      <c r="B3920" s="22">
+      <c r="B3920" s="21">
         <v>8.067465871936125E-5</v>
       </c>
-      <c r="C3920" s="22">
+      <c r="C3920" s="21">
         <v>-3.5374377477465149E-5</v>
       </c>
-      <c r="D3920" s="22">
+      <c r="D3920" s="21">
         <v>4.5300281241896101E-5</v>
       </c>
     </row>
@@ -58647,13 +58657,13 @@
       <c r="A3921" s="1">
         <v>44435</v>
       </c>
-      <c r="B3921" s="22">
+      <c r="B3921" s="21">
         <v>-2.2471315458773804E-4</v>
       </c>
-      <c r="C3921" s="22">
+      <c r="C3921" s="21">
         <v>5.9130792801814748E-5</v>
       </c>
-      <c r="D3921" s="22">
+      <c r="D3921" s="21">
         <v>-1.655823617859233E-4</v>
       </c>
     </row>
@@ -58661,13 +58671,13 @@
       <c r="A3922" s="1">
         <v>44438</v>
       </c>
-      <c r="B3922" s="22">
+      <c r="B3922" s="21">
         <v>-4.0714887582378197E-5</v>
       </c>
-      <c r="C3922" s="22">
+      <c r="C3922" s="21">
         <v>1.6532012780547149E-5</v>
       </c>
-      <c r="D3922" s="22">
+      <c r="D3922" s="21">
         <v>-2.4182874801831048E-5</v>
       </c>
     </row>
@@ -58675,14 +58685,308 @@
       <c r="A3923" s="1">
         <v>44439</v>
       </c>
-      <c r="B3923" s="22">
+      <c r="B3923" s="21">
         <v>1.398031116106215E-6</v>
       </c>
-      <c r="C3923" s="22">
+      <c r="C3923" s="21">
         <v>7.2071381024905053E-6</v>
       </c>
-      <c r="D3923" s="22">
+      <c r="D3923" s="21">
         <v>8.6051692185967205E-6</v>
+      </c>
+    </row>
+    <row r="3924" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3924" s="1">
+        <v>44440</v>
+      </c>
+      <c r="B3924" s="21">
+        <v>-7.7263484640244245E-5</v>
+      </c>
+      <c r="C3924" s="21">
+        <v>5.2057264260225078E-4</v>
+      </c>
+      <c r="D3924" s="21">
+        <v>4.4330915796200656E-4</v>
+      </c>
+    </row>
+    <row r="3925" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3925" s="1">
+        <v>44441</v>
+      </c>
+      <c r="B3925" s="21">
+        <v>-1.3450079774133552E-3</v>
+      </c>
+      <c r="C3925" s="21">
+        <v>3.5419299833280436E-4</v>
+      </c>
+      <c r="D3925" s="21">
+        <v>-9.9081497908055081E-4</v>
+      </c>
+    </row>
+    <row r="3926" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3926" s="1">
+        <v>44442</v>
+      </c>
+      <c r="B3926" s="21">
+        <v>7.5331668122622129E-5</v>
+      </c>
+      <c r="C3926" s="21">
+        <v>-4.4569117466661309E-5</v>
+      </c>
+      <c r="D3926" s="21">
+        <v>3.0762550655960819E-5</v>
+      </c>
+    </row>
+    <row r="3927" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3927" s="1">
+        <v>44446</v>
+      </c>
+      <c r="B3927" s="21">
+        <v>1.4077026080276962E-3</v>
+      </c>
+      <c r="C3927" s="21">
+        <v>-8.3985583685539978E-4</v>
+      </c>
+      <c r="D3927" s="21">
+        <v>5.6784677117229637E-4</v>
+      </c>
+    </row>
+    <row r="3928" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3928" s="1">
+        <v>44447</v>
+      </c>
+      <c r="B3928" s="21">
+        <v>6.4257846974287089E-4</v>
+      </c>
+      <c r="C3928" s="21">
+        <v>4.4083945056159927E-5</v>
+      </c>
+      <c r="D3928" s="21">
+        <v>6.8666241479903084E-4</v>
+      </c>
+    </row>
+    <row r="3929" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3929" s="1">
+        <v>44448</v>
+      </c>
+      <c r="B3929" s="21">
+        <v>2.0274773421293611E-3</v>
+      </c>
+      <c r="C3929" s="21">
+        <v>-7.6363909484204219E-4</v>
+      </c>
+      <c r="D3929" s="21">
+        <v>1.2638382472873189E-3</v>
+      </c>
+    </row>
+    <row r="3930" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3930" s="1">
+        <v>44449</v>
+      </c>
+      <c r="B3930" s="21">
+        <v>3.5664165708636404E-3</v>
+      </c>
+      <c r="C3930" s="21">
+        <v>-1.4942173199313177E-3</v>
+      </c>
+      <c r="D3930" s="21">
+        <v>2.0721992509323229E-3</v>
+      </c>
+    </row>
+    <row r="3931" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3931" s="1">
+        <v>44452</v>
+      </c>
+      <c r="B3931" s="21">
+        <v>-1.1705950108166416E-3</v>
+      </c>
+      <c r="C3931" s="21">
+        <v>1.4172168967777987E-3</v>
+      </c>
+      <c r="D3931" s="21">
+        <v>2.4662188596115712E-4</v>
+      </c>
+    </row>
+    <row r="3932" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3932" s="1">
+        <v>44453</v>
+      </c>
+      <c r="B3932" s="21">
+        <v>2.7024315647642158E-3</v>
+      </c>
+      <c r="C3932" s="21">
+        <v>-4.9897799267106639E-4</v>
+      </c>
+      <c r="D3932" s="21">
+        <v>2.2034535720931495E-3</v>
+      </c>
+    </row>
+    <row r="3933" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3933" s="1">
+        <v>44454</v>
+      </c>
+      <c r="B3933" s="21">
+        <v>-4.3557810921152447E-3</v>
+      </c>
+      <c r="C3933" s="21">
+        <v>1.795333458692303E-3</v>
+      </c>
+      <c r="D3933" s="21">
+        <v>-2.5604476334229417E-3</v>
+      </c>
+    </row>
+    <row r="3934" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3934" s="1">
+        <v>44455</v>
+      </c>
+      <c r="B3934" s="21">
+        <v>8.3887276027657482E-4</v>
+      </c>
+      <c r="C3934" s="21">
+        <v>-1.9927819875830552E-4</v>
+      </c>
+      <c r="D3934" s="21">
+        <v>6.3959456151826933E-4</v>
+      </c>
+    </row>
+    <row r="3935" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3935" s="1">
+        <v>44456</v>
+      </c>
+      <c r="B3935" s="21">
+        <v>4.6838068807287551E-3</v>
+      </c>
+      <c r="C3935" s="21">
+        <v>-2.4891924867823084E-3</v>
+      </c>
+      <c r="D3935" s="21">
+        <v>2.1946143939464468E-3</v>
+      </c>
+    </row>
+    <row r="3936" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3936" s="1">
+        <v>44459</v>
+      </c>
+      <c r="B3936" s="21">
+        <v>9.0607914572606099E-3</v>
+      </c>
+      <c r="C3936" s="21">
+        <v>-5.8324783299493442E-3</v>
+      </c>
+      <c r="D3936" s="21">
+        <v>3.2283131273112657E-3</v>
+      </c>
+    </row>
+    <row r="3937" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3937" s="1">
+        <v>44460</v>
+      </c>
+      <c r="B3937" s="21">
+        <v>7.0125035827137583E-4</v>
+      </c>
+      <c r="C3937" s="21">
+        <v>1.0256501605030537E-3</v>
+      </c>
+      <c r="D3937" s="21">
+        <v>1.7269005187744296E-3</v>
+      </c>
+    </row>
+    <row r="3938" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3938" s="1">
+        <v>44461</v>
+      </c>
+      <c r="B3938" s="21">
+        <v>-5.8252150179383573E-3</v>
+      </c>
+      <c r="C3938" s="21">
+        <v>4.8128948892325087E-3</v>
+      </c>
+      <c r="D3938" s="21">
+        <v>-1.0123201287058486E-3</v>
+      </c>
+    </row>
+    <row r="3939" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3939" s="1">
+        <v>44462</v>
+      </c>
+      <c r="B3939" s="21">
+        <v>-7.1543544864894953E-3</v>
+      </c>
+      <c r="C3939" s="21">
+        <v>3.2371103352444963E-3</v>
+      </c>
+      <c r="D3939" s="21">
+        <v>-3.9172441512449994E-3</v>
+      </c>
+    </row>
+    <row r="3940" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3940" s="1">
+        <v>44463</v>
+      </c>
+      <c r="B3940" s="21">
+        <v>-9.1393073197222922E-4</v>
+      </c>
+      <c r="C3940" s="21">
+        <v>8.187130755390056E-4</v>
+      </c>
+      <c r="D3940" s="21">
+        <v>-9.5217656433223621E-5</v>
+      </c>
+    </row>
+    <row r="3941" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3941" s="1">
+        <v>44466</v>
+      </c>
+      <c r="B3941" s="21">
+        <v>1.4872558902672979E-3</v>
+      </c>
+      <c r="C3941" s="21">
+        <v>-5.07202174518886E-4</v>
+      </c>
+      <c r="D3941" s="21">
+        <v>9.8005371574841176E-4</v>
+      </c>
+    </row>
+    <row r="3942" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3942" s="1">
+        <v>44467</v>
+      </c>
+      <c r="B3942" s="21">
+        <v>1.0835256480439358E-2</v>
+      </c>
+      <c r="C3942" s="21">
+        <v>-5.107055510526478E-3</v>
+      </c>
+      <c r="D3942" s="21">
+        <v>5.7282009699128802E-3</v>
+      </c>
+    </row>
+    <row r="3943" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3943" s="1">
+        <v>44468</v>
+      </c>
+      <c r="B3943" s="21">
+        <v>-9.025454244973968E-4</v>
+      </c>
+      <c r="C3943" s="21">
+        <v>7.4508265440231401E-4</v>
+      </c>
+      <c r="D3943" s="21">
+        <v>-1.5746277009508279E-4</v>
+      </c>
+    </row>
+    <row r="3944" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3944" s="1">
+        <v>44469</v>
+      </c>
+      <c r="B3944" s="21">
+        <v>7.3941226221983626E-3</v>
+      </c>
+      <c r="C3944" s="21">
+        <v>-2.0780297910211582E-3</v>
+      </c>
+      <c r="D3944" s="21">
+        <v>5.3160928311772049E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update returns data for end of year
</commit_message>
<xml_diff>
--- a/EquityHedging/data/update_strats/put_spread_data.xlsx
+++ b/EquityHedging/data/update_strats/put_spread_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NVG9HXP\Documents\Projects\RMP\EquityHedging\data\update_strats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B6B1EF4-EFB0-4DA8-81D1-925076944B65}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{61AB66A9-3E43-4DB8-A127-848294BE46B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="3" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <definedName name="solver_typ" hidden="1">3</definedName>
     <definedName name="solver_val" hidden="1">0</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,12 +43,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Put Spread</t>
-  </si>
-  <si>
-    <t>Source: Bloomberg Barclays, NISA Calculations</t>
   </si>
   <si>
     <t>Short 90 Put</t>
@@ -73,6 +70,12 @@
   </si>
   <si>
     <t>Disclaimer</t>
+  </si>
+  <si>
+    <t>Source: Bloomberg, NISA Calculations</t>
+  </si>
+  <si>
+    <t>As of December 31, 2021</t>
   </si>
 </sst>
 </file>
@@ -1012,7 +1015,9 @@
   </sheetPr>
   <dimension ref="B9:B25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1023,7 +1028,7 @@
     <row r="9" spans="2:2" ht="80.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="2:2" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B16" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="23.25" x14ac:dyDescent="0.35">
@@ -1037,12 +1042,12 @@
     </row>
     <row r="20" spans="2:2" ht="20.25" x14ac:dyDescent="0.25">
       <c r="B20" s="16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B21" s="22">
-        <v>44500</v>
+      <c r="B21" s="22" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
@@ -1057,7 +1062,7 @@
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="18" t="str">
         <f ca="1">CONCATENATE("© ",YEAR(TODAY())," NISA Investment Advisors, LLC. All rights reserved.")</f>
-        <v>© 2021 NISA Investment Advisors, LLC. All rights reserved.</v>
+        <v>© 2022 NISA Investment Advisors, LLC. All rights reserved.</v>
       </c>
     </row>
   </sheetData>
@@ -1072,11 +1077,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D193"/>
+  <dimension ref="A1:D195"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A193" sqref="A193"/>
+      <pane ySplit="2" topLeftCell="A172" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A175" sqref="A175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,19 +1095,19 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3777,6 +3782,34 @@
       </c>
       <c r="D193" s="12">
         <v>-2.4750470084351051E-2</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" s="1">
+        <v>44530</v>
+      </c>
+      <c r="B194" s="12">
+        <v>-6.3705138367804448E-3</v>
+      </c>
+      <c r="C194" s="12">
+        <v>1.6813280838404721E-3</v>
+      </c>
+      <c r="D194" s="12">
+        <v>-4.6891857529399728E-3</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" s="1">
+        <v>44561</v>
+      </c>
+      <c r="B195" s="12">
+        <v>-2.0488144916505857E-2</v>
+      </c>
+      <c r="C195" s="12">
+        <v>1.3328654361829506E-2</v>
+      </c>
+      <c r="D195" s="12">
+        <v>-7.159490554676351E-3</v>
       </c>
     </row>
   </sheetData>
@@ -3786,11 +3819,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D3965"/>
+  <dimension ref="A1:D4008"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3930" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3965" sqref="B3965"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3487" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3801,15 +3834,15 @@
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>0</v>
@@ -59295,6 +59328,608 @@
       </c>
       <c r="D3965" s="21">
         <v>-3.7141842528592094E-4</v>
+      </c>
+    </row>
+    <row r="3966" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3966" s="1">
+        <v>44501</v>
+      </c>
+      <c r="B3966" s="21">
+        <v>-5.1983046677795048E-4</v>
+      </c>
+      <c r="C3966" s="21">
+        <v>3.7589652929190649E-4</v>
+      </c>
+      <c r="D3966" s="21">
+        <v>-1.4393393748604399E-4</v>
+      </c>
+    </row>
+    <row r="3967" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3967" s="1">
+        <v>44502</v>
+      </c>
+      <c r="B3967" s="21">
+        <v>-1.0038591831433644E-3</v>
+      </c>
+      <c r="C3967" s="21">
+        <v>2.2072844279267197E-4</v>
+      </c>
+      <c r="D3967" s="21">
+        <v>-7.8313074035069236E-4</v>
+      </c>
+    </row>
+    <row r="3968" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3968" s="1">
+        <v>44503</v>
+      </c>
+      <c r="B3968" s="21">
+        <v>-1.4461071158315901E-3</v>
+      </c>
+      <c r="C3968" s="21">
+        <v>2.7721485499798893E-4</v>
+      </c>
+      <c r="D3968" s="21">
+        <v>-1.1688922608336012E-3</v>
+      </c>
+    </row>
+    <row r="3969" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3969" s="1">
+        <v>44504</v>
+      </c>
+      <c r="B3969" s="21">
+        <v>-8.3295396259557952E-4</v>
+      </c>
+      <c r="C3969" s="21">
+        <v>-1.0833894861064251E-5</v>
+      </c>
+      <c r="D3969" s="21">
+        <v>-8.437878574566438E-4</v>
+      </c>
+    </row>
+    <row r="3970" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3970" s="1">
+        <v>44505</v>
+      </c>
+      <c r="B3970" s="21">
+        <v>-5.911525433163773E-4</v>
+      </c>
+      <c r="C3970" s="21">
+        <v>-8.8754068546124571E-5</v>
+      </c>
+      <c r="D3970" s="21">
+        <v>-6.7990661186250183E-4</v>
+      </c>
+    </row>
+    <row r="3971" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3971" s="1">
+        <v>44508</v>
+      </c>
+      <c r="B3971" s="21">
+        <v>-1.2709438490485274E-4</v>
+      </c>
+      <c r="C3971" s="21">
+        <v>8.8452667302277494E-5</v>
+      </c>
+      <c r="D3971" s="21">
+        <v>-3.8641717602575247E-5</v>
+      </c>
+    </row>
+    <row r="3972" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3972" s="1">
+        <v>44509</v>
+      </c>
+      <c r="B3972" s="21">
+        <v>4.9005987937639293E-4</v>
+      </c>
+      <c r="C3972" s="21">
+        <v>1.1111197941620445E-5</v>
+      </c>
+      <c r="D3972" s="21">
+        <v>5.0117107731801334E-4</v>
+      </c>
+    </row>
+    <row r="3973" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3973" s="1">
+        <v>44510</v>
+      </c>
+      <c r="B3973" s="21">
+        <v>1.254165919067782E-3</v>
+      </c>
+      <c r="C3973" s="21">
+        <v>-5.5223672175935941E-5</v>
+      </c>
+      <c r="D3973" s="21">
+        <v>1.1989422468918461E-3</v>
+      </c>
+    </row>
+    <row r="3974" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3974" s="1">
+        <v>44511</v>
+      </c>
+      <c r="B3974" s="21">
+        <v>-4.251996684467848E-5</v>
+      </c>
+      <c r="C3974" s="21">
+        <v>2.4873662858838517E-4</v>
+      </c>
+      <c r="D3974" s="21">
+        <v>2.0621666174370668E-4</v>
+      </c>
+    </row>
+    <row r="3975" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3975" s="1">
+        <v>44512</v>
+      </c>
+      <c r="B3975" s="21">
+        <v>-1.3342589188056273E-3</v>
+      </c>
+      <c r="C3975" s="21">
+        <v>2.2620073978880869E-4</v>
+      </c>
+      <c r="D3975" s="21">
+        <v>-1.1080581790168186E-3</v>
+      </c>
+    </row>
+    <row r="3976" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3976" s="1">
+        <v>44515</v>
+      </c>
+      <c r="B3976" s="21">
+        <v>-1.8094213381020813E-5</v>
+      </c>
+      <c r="C3976" s="21">
+        <v>1.4876316202726346E-4</v>
+      </c>
+      <c r="D3976" s="21">
+        <v>1.3066894864624263E-4</v>
+      </c>
+    </row>
+    <row r="3977" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3977" s="1">
+        <v>44516</v>
+      </c>
+      <c r="B3977" s="21">
+        <v>-3.4602542745556321E-4</v>
+      </c>
+      <c r="C3977" s="21">
+        <v>4.4176675080477181E-5</v>
+      </c>
+      <c r="D3977" s="21">
+        <v>-3.0184875237508602E-4</v>
+      </c>
+    </row>
+    <row r="3978" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3978" s="1">
+        <v>44517</v>
+      </c>
+      <c r="B3978" s="21">
+        <v>1.6132223425855443E-4</v>
+      </c>
+      <c r="C3978" s="21">
+        <v>1.6925053242459755E-5</v>
+      </c>
+      <c r="D3978" s="21">
+        <v>1.7824728750101418E-4</v>
+      </c>
+    </row>
+    <row r="3979" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3979" s="1">
+        <v>44518</v>
+      </c>
+      <c r="B3979" s="21">
+        <v>-2.5448682057684682E-4</v>
+      </c>
+      <c r="C3979" s="21">
+        <v>1.0940139742017964E-5</v>
+      </c>
+      <c r="D3979" s="21">
+        <v>-2.4354668083482887E-4</v>
+      </c>
+    </row>
+    <row r="3980" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3980" s="1">
+        <v>44519</v>
+      </c>
+      <c r="B3980" s="21">
+        <v>9.9794238949120202E-5</v>
+      </c>
+      <c r="C3980" s="21">
+        <v>1.0928431428659161E-5</v>
+      </c>
+      <c r="D3980" s="21">
+        <v>1.1072267037777936E-4</v>
+      </c>
+    </row>
+    <row r="3981" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3981" s="1">
+        <v>44522</v>
+      </c>
+      <c r="B3981" s="21">
+        <v>1.9108122692028438E-4</v>
+      </c>
+      <c r="C3981" s="21">
+        <v>1.1267844095735109E-5</v>
+      </c>
+      <c r="D3981" s="21">
+        <v>2.023490710160195E-4</v>
+      </c>
+    </row>
+    <row r="3982" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3982" s="1">
+        <v>44523</v>
+      </c>
+      <c r="B3982" s="21">
+        <v>-1.149826653974551E-4</v>
+      </c>
+      <c r="C3982" s="21">
+        <v>4.4269772724729661E-5</v>
+      </c>
+      <c r="D3982" s="21">
+        <v>-7.0712892672725435E-5</v>
+      </c>
+    </row>
+    <row r="3983" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3983" s="1">
+        <v>44524</v>
+      </c>
+      <c r="B3983" s="21">
+        <v>-1.2631949705269499E-4</v>
+      </c>
+      <c r="C3983" s="21">
+        <v>6.049142053003068E-5</v>
+      </c>
+      <c r="D3983" s="21">
+        <v>-6.5828076522664311E-5</v>
+      </c>
+    </row>
+    <row r="3984" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3984" s="1">
+        <v>44526</v>
+      </c>
+      <c r="B3984" s="21">
+        <v>6.7322942404548808E-4</v>
+      </c>
+      <c r="C3984" s="21">
+        <v>-3.7978002944742906E-4</v>
+      </c>
+      <c r="D3984" s="21">
+        <v>2.9344939459805902E-4</v>
+      </c>
+    </row>
+    <row r="3985" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3985" s="1">
+        <v>44529</v>
+      </c>
+      <c r="B3985" s="21">
+        <v>-2.615992726457269E-3</v>
+      </c>
+      <c r="C3985" s="21">
+        <v>4.1853632466110882E-4</v>
+      </c>
+      <c r="D3985" s="21">
+        <v>-2.1974564017961601E-3</v>
+      </c>
+    </row>
+    <row r="3986" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3986" s="1">
+        <v>44530</v>
+      </c>
+      <c r="B3986" s="21">
+        <v>1.2095123142129021E-4</v>
+      </c>
+      <c r="C3986" s="21">
+        <v>2.4229759127208656E-7</v>
+      </c>
+      <c r="D3986" s="21">
+        <v>1.211935290125623E-4</v>
+      </c>
+    </row>
+    <row r="3987" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3987" s="1">
+        <v>44531</v>
+      </c>
+      <c r="B3987" s="21">
+        <v>5.554168479380458E-3</v>
+      </c>
+      <c r="C3987" s="21">
+        <v>-4.2397935174909871E-3</v>
+      </c>
+      <c r="D3987" s="21">
+        <v>1.3143749618894709E-3</v>
+      </c>
+    </row>
+    <row r="3988" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3988" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B3988" s="21">
+        <v>-7.1246861742272939E-3</v>
+      </c>
+      <c r="C3988" s="21">
+        <v>3.3545182481579993E-3</v>
+      </c>
+      <c r="D3988" s="21">
+        <v>-3.7701679260692946E-3</v>
+      </c>
+    </row>
+    <row r="3989" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3989" s="1">
+        <v>44533</v>
+      </c>
+      <c r="B3989" s="21">
+        <v>3.7013535408111022E-3</v>
+      </c>
+      <c r="C3989" s="21">
+        <v>-3.3318343541591526E-3</v>
+      </c>
+      <c r="D3989" s="21">
+        <v>3.6951918665194955E-4</v>
+      </c>
+    </row>
+    <row r="3990" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3990" s="1">
+        <v>44536</v>
+      </c>
+      <c r="B3990" s="21">
+        <v>-5.3667877137525419E-3</v>
+      </c>
+      <c r="C3990" s="21">
+        <v>5.0045529298576421E-3</v>
+      </c>
+      <c r="D3990" s="21">
+        <v>-3.6223478389489985E-4</v>
+      </c>
+    </row>
+    <row r="3991" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3991" s="1">
+        <v>44537</v>
+      </c>
+      <c r="B3991" s="21">
+        <v>-8.874750727329489E-3</v>
+      </c>
+      <c r="C3991" s="21">
+        <v>5.7458884652001087E-3</v>
+      </c>
+      <c r="D3991" s="21">
+        <v>-3.1288622621293803E-3</v>
+      </c>
+    </row>
+    <row r="3992" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3992" s="1">
+        <v>44538</v>
+      </c>
+      <c r="B3992" s="21">
+        <v>-1.0311385452543502E-3</v>
+      </c>
+      <c r="C3992" s="21">
+        <v>1.5222160234692427E-3</v>
+      </c>
+      <c r="D3992" s="21">
+        <v>4.9107747821489252E-4</v>
+      </c>
+    </row>
+    <row r="3993" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3993" s="1">
+        <v>44539</v>
+      </c>
+      <c r="B3993" s="21">
+        <v>2.3579031704777246E-3</v>
+      </c>
+      <c r="C3993" s="21">
+        <v>-1.3250952434484139E-3</v>
+      </c>
+      <c r="D3993" s="21">
+        <v>1.0328079270293107E-3</v>
+      </c>
+    </row>
+    <row r="3994" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3994" s="1">
+        <v>44540</v>
+      </c>
+      <c r="B3994" s="21">
+        <v>-3.4463562245906445E-3</v>
+      </c>
+      <c r="C3994" s="21">
+        <v>1.9587842103661966E-3</v>
+      </c>
+      <c r="D3994" s="21">
+        <v>-1.4875720142244479E-3</v>
+      </c>
+    </row>
+    <row r="3995" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3995" s="1">
+        <v>44543</v>
+      </c>
+      <c r="B3995" s="21">
+        <v>3.0674593057596193E-3</v>
+      </c>
+      <c r="C3995" s="21">
+        <v>-1.0208659689772989E-3</v>
+      </c>
+      <c r="D3995" s="21">
+        <v>2.0465933367823201E-3</v>
+      </c>
+    </row>
+    <row r="3996" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3996" s="1">
+        <v>44544</v>
+      </c>
+      <c r="B3996" s="21">
+        <v>2.435467137836822E-3</v>
+      </c>
+      <c r="C3996" s="21">
+        <v>-1.4789509535879431E-3</v>
+      </c>
+      <c r="D3996" s="21">
+        <v>9.5651618424887888E-4</v>
+      </c>
+    </row>
+    <row r="3997" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3997" s="1">
+        <v>44545</v>
+      </c>
+      <c r="B3997" s="21">
+        <v>-6.1354722142608134E-3</v>
+      </c>
+      <c r="C3997" s="21">
+        <v>3.1135505333913485E-3</v>
+      </c>
+      <c r="D3997" s="21">
+        <v>-3.0219216808694649E-3</v>
+      </c>
+    </row>
+    <row r="3998" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3998" s="1">
+        <v>44546</v>
+      </c>
+      <c r="B3998" s="21">
+        <v>2.8755184650286884E-3</v>
+      </c>
+      <c r="C3998" s="21">
+        <v>-1.204741808357455E-3</v>
+      </c>
+      <c r="D3998" s="21">
+        <v>1.6707766566712334E-3</v>
+      </c>
+    </row>
+    <row r="3999" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3999" s="1">
+        <v>44547</v>
+      </c>
+      <c r="B3999" s="21">
+        <v>3.7725535204046487E-3</v>
+      </c>
+      <c r="C3999" s="21">
+        <v>-1.5102083123864601E-3</v>
+      </c>
+      <c r="D3999" s="21">
+        <v>2.2623452080181884E-3</v>
+      </c>
+    </row>
+    <row r="4000" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4000" s="1">
+        <v>44550</v>
+      </c>
+      <c r="B4000" s="21">
+        <v>4.4198475851728808E-3</v>
+      </c>
+      <c r="C4000" s="21">
+        <v>-1.1866596295621102E-3</v>
+      </c>
+      <c r="D4000" s="21">
+        <v>3.2331879556107704E-3</v>
+      </c>
+    </row>
+    <row r="4001" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4001" s="1">
+        <v>44551</v>
+      </c>
+      <c r="B4001" s="21">
+        <v>-7.859486176001752E-3</v>
+      </c>
+      <c r="C4001" s="21">
+        <v>2.7675728542463527E-3</v>
+      </c>
+      <c r="D4001" s="21">
+        <v>-5.0919133217553992E-3</v>
+      </c>
+    </row>
+    <row r="4002" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4002" s="1">
+        <v>44552</v>
+      </c>
+      <c r="B4002" s="21">
+        <v>-3.6571075283826902E-3</v>
+      </c>
+      <c r="C4002" s="21">
+        <v>2.0977122150049828E-3</v>
+      </c>
+      <c r="D4002" s="21">
+        <v>-1.5593953133777073E-3</v>
+      </c>
+    </row>
+    <row r="4003" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4003" s="1">
+        <v>44553</v>
+      </c>
+      <c r="B4003" s="21">
+        <v>-2.0865593943839135E-3</v>
+      </c>
+      <c r="C4003" s="21">
+        <v>7.6941739719527851E-4</v>
+      </c>
+      <c r="D4003" s="21">
+        <v>-1.317141997188635E-3</v>
+      </c>
+    </row>
+    <row r="4004" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4004" s="1">
+        <v>44557</v>
+      </c>
+      <c r="B4004" s="21">
+        <v>-4.2998201716750806E-3</v>
+      </c>
+      <c r="C4004" s="21">
+        <v>1.4090298444950787E-3</v>
+      </c>
+      <c r="D4004" s="21">
+        <v>-2.8907903271800017E-3</v>
+      </c>
+    </row>
+    <row r="4005" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4005" s="1">
+        <v>44558</v>
+      </c>
+      <c r="B4005" s="21">
+        <v>1.9785021936998709E-4</v>
+      </c>
+      <c r="C4005" s="21">
+        <v>2.7043381491242643E-4</v>
+      </c>
+      <c r="D4005" s="21">
+        <v>4.6828403428241351E-4</v>
+      </c>
+    </row>
+    <row r="4006" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4006" s="1">
+        <v>44559</v>
+      </c>
+      <c r="B4006" s="21">
+        <v>-3.0899110541981773E-4</v>
+      </c>
+      <c r="C4006" s="21">
+        <v>4.7557853257574516E-4</v>
+      </c>
+      <c r="D4006" s="21">
+        <v>1.6658742715592743E-4</v>
+      </c>
+    </row>
+    <row r="4007" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4007" s="1">
+        <v>44560</v>
+      </c>
+      <c r="B4007" s="21">
+        <v>6.1296223122554445E-4</v>
+      </c>
+      <c r="C4007" s="21">
+        <v>1.0757317481667663E-5</v>
+      </c>
+      <c r="D4007" s="21">
+        <v>6.2371954870721216E-4</v>
+      </c>
+    </row>
+    <row r="4008" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4008" s="1">
+        <v>44561</v>
+      </c>
+      <c r="B4008" s="21">
+        <v>7.0338825026686409E-4</v>
+      </c>
+      <c r="C4008" s="21">
+        <v>1.0830334680480304E-4</v>
+      </c>
+      <c r="D4008" s="21">
+        <v>8.1169159707166708E-4</v>
       </c>
     </row>
   </sheetData>
@@ -59509,7 +60144,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update put spread and vrr data to 1/31/2022
</commit_message>
<xml_diff>
--- a/EquityHedging/data/update_strats/put_spread_data.xlsx
+++ b/EquityHedging/data/update_strats/put_spread_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NVG9HXP\Documents\Projects\RMP\EquityHedging\data\update_strats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61AB66A9-3E43-4DB8-A127-848294BE46B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D302A8E4-E04F-4342-AF75-CFB8841E25F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="3" r:id="rId1"/>
@@ -75,7 +75,7 @@
     <t>Source: Bloomberg, NISA Calculations</t>
   </si>
   <si>
-    <t>As of December 31, 2021</t>
+    <t>As of January 31, 2022</t>
   </si>
 </sst>
 </file>
@@ -1015,9 +1015,7 @@
   </sheetPr>
   <dimension ref="B9:B25"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1077,11 +1075,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D195"/>
+  <dimension ref="A1:D196"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A172" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A175" sqref="A175"/>
+      <pane ySplit="2" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3812,6 +3810,20 @@
         <v>-7.159490554676351E-3</v>
       </c>
     </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196" s="1">
+        <v>44592</v>
+      </c>
+      <c r="B196" s="12">
+        <v>1.1108743132965948E-2</v>
+      </c>
+      <c r="C196" s="12">
+        <v>-1.2407495733441909E-3</v>
+      </c>
+      <c r="D196" s="12">
+        <v>9.8679935596217572E-3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3819,17 +3831,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D4008"/>
+  <dimension ref="A1:F4027"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3487" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3995" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4027" sqref="A4027"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="9.140625" style="2"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -59820,7 +59833,7 @@
         <v>3.2331879556107704E-3</v>
       </c>
     </row>
-    <row r="4001" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4001" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4001" s="1">
         <v>44551</v>
       </c>
@@ -59834,7 +59847,7 @@
         <v>-5.0919133217553992E-3</v>
       </c>
     </row>
-    <row r="4002" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4002" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4002" s="1">
         <v>44552</v>
       </c>
@@ -59848,7 +59861,7 @@
         <v>-1.5593953133777073E-3</v>
       </c>
     </row>
-    <row r="4003" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4003" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4003" s="1">
         <v>44553</v>
       </c>
@@ -59862,7 +59875,7 @@
         <v>-1.317141997188635E-3</v>
       </c>
     </row>
-    <row r="4004" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4004" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4004" s="1">
         <v>44557</v>
       </c>
@@ -59876,7 +59889,7 @@
         <v>-2.8907903271800017E-3</v>
       </c>
     </row>
-    <row r="4005" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4005" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4005" s="1">
         <v>44558</v>
       </c>
@@ -59890,7 +59903,7 @@
         <v>4.6828403428241351E-4</v>
       </c>
     </row>
-    <row r="4006" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4006" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4006" s="1">
         <v>44559</v>
       </c>
@@ -59904,7 +59917,7 @@
         <v>1.6658742715592743E-4</v>
       </c>
     </row>
-    <row r="4007" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4007" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4007" s="1">
         <v>44560</v>
       </c>
@@ -59918,7 +59931,7 @@
         <v>6.2371954870721216E-4</v>
       </c>
     </row>
-    <row r="4008" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4008" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4008" s="1">
         <v>44561</v>
       </c>
@@ -59930,6 +59943,274 @@
       </c>
       <c r="D4008" s="21">
         <v>8.1169159707166708E-4</v>
+      </c>
+    </row>
+    <row r="4009" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4009" s="1">
+        <v>44564</v>
+      </c>
+      <c r="B4009" s="21">
+        <v>-1.401728044659287E-3</v>
+      </c>
+      <c r="C4009" s="21">
+        <v>6.7873943944693493E-4</v>
+      </c>
+      <c r="D4009" s="21">
+        <v>-7.2298860521235206E-4</v>
+      </c>
+      <c r="E4009" s="21"/>
+      <c r="F4009" s="21"/>
+    </row>
+    <row r="4010" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4010" s="1">
+        <v>44565</v>
+      </c>
+      <c r="B4010" s="21">
+        <v>8.0976150987871557E-5</v>
+      </c>
+      <c r="C4010" s="21">
+        <v>-2.1576254018356383E-5</v>
+      </c>
+      <c r="D4010" s="21">
+        <v>5.9399896969515175E-5</v>
+      </c>
+    </row>
+    <row r="4011" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4011" s="1">
+        <v>44566</v>
+      </c>
+      <c r="B4011" s="21">
+        <v>4.2859785573988044E-3</v>
+      </c>
+      <c r="C4011" s="21">
+        <v>-1.6206820828756625E-3</v>
+      </c>
+      <c r="D4011" s="21">
+        <v>2.6652964745231419E-3</v>
+      </c>
+    </row>
+    <row r="4012" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4012" s="1">
+        <v>44567</v>
+      </c>
+      <c r="B4012" s="21">
+        <v>3.165303789982992E-4</v>
+      </c>
+      <c r="C4012" s="21">
+        <v>1.2050482859636265E-4</v>
+      </c>
+      <c r="D4012" s="21">
+        <v>4.3703520759466184E-4</v>
+      </c>
+    </row>
+    <row r="4013" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4013" s="1">
+        <v>44568</v>
+      </c>
+      <c r="B4013" s="21">
+        <v>1.274516342572017E-3</v>
+      </c>
+      <c r="C4013" s="21">
+        <v>3.2895643077266508E-4</v>
+      </c>
+      <c r="D4013" s="21">
+        <v>1.603472773344682E-3</v>
+      </c>
+    </row>
+    <row r="4014" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4014" s="1">
+        <v>44571</v>
+      </c>
+      <c r="B4014" s="21">
+        <v>3.7172108328854863E-4</v>
+      </c>
+      <c r="C4014" s="21">
+        <v>1.8623053413966388E-4</v>
+      </c>
+      <c r="D4014" s="21">
+        <v>5.579516174282125E-4</v>
+      </c>
+    </row>
+    <row r="4015" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4015" s="1">
+        <v>44572</v>
+      </c>
+      <c r="B4015" s="21">
+        <v>-2.9138273518746196E-3</v>
+      </c>
+      <c r="C4015" s="21">
+        <v>8.1117997499457952E-4</v>
+      </c>
+      <c r="D4015" s="21">
+        <v>-2.1026473768800402E-3</v>
+      </c>
+    </row>
+    <row r="4016" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4016" s="1">
+        <v>44573</v>
+      </c>
+      <c r="B4016" s="21">
+        <v>-6.5498819887711672E-4</v>
+      </c>
+      <c r="C4016" s="21">
+        <v>5.148438528770129E-4</v>
+      </c>
+      <c r="D4016" s="21">
+        <v>-1.4014434600010382E-4</v>
+      </c>
+    </row>
+    <row r="4017" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4017" s="1">
+        <v>44574</v>
+      </c>
+      <c r="B4017" s="21">
+        <v>3.4555480445034137E-3</v>
+      </c>
+      <c r="C4017" s="21">
+        <v>-1.4652506712739791E-3</v>
+      </c>
+      <c r="D4017" s="21">
+        <v>1.9902973732294346E-3</v>
+      </c>
+    </row>
+    <row r="4018" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4018" s="1">
+        <v>44575</v>
+      </c>
+      <c r="B4018" s="21">
+        <v>-1.9478474157242517E-4</v>
+      </c>
+      <c r="C4018" s="21">
+        <v>7.566560876640882E-4</v>
+      </c>
+      <c r="D4018" s="21">
+        <v>5.6187134609166306E-4</v>
+      </c>
+    </row>
+    <row r="4019" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4019" s="1">
+        <v>44579</v>
+      </c>
+      <c r="B4019" s="21">
+        <v>5.6510253801592822E-3</v>
+      </c>
+      <c r="C4019" s="21">
+        <v>-1.9168454274513171E-3</v>
+      </c>
+      <c r="D4019" s="21">
+        <v>3.7341799527079653E-3</v>
+      </c>
+    </row>
+    <row r="4020" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4020" s="1">
+        <v>44581</v>
+      </c>
+      <c r="B4020" s="21">
+        <v>8.7153095779378947E-3</v>
+      </c>
+      <c r="C4020" s="21">
+        <v>-3.1048208897116306E-3</v>
+      </c>
+      <c r="D4020" s="21">
+        <v>5.6104886882262645E-3</v>
+      </c>
+    </row>
+    <row r="4021" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4021" s="1">
+        <v>44582</v>
+      </c>
+      <c r="B4021" s="21">
+        <v>1.0090916718238549E-2</v>
+      </c>
+      <c r="C4021" s="21">
+        <v>-3.9513304948456058E-3</v>
+      </c>
+      <c r="D4021" s="21">
+        <v>6.1395862233929429E-3</v>
+      </c>
+    </row>
+    <row r="4022" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4022" s="1">
+        <v>44585</v>
+      </c>
+      <c r="B4022" s="21">
+        <v>-1.9404974821356543E-3</v>
+      </c>
+      <c r="C4022" s="21">
+        <v>4.4806197271988801E-4</v>
+      </c>
+      <c r="D4022" s="21">
+        <v>-1.4924355094157664E-3</v>
+      </c>
+    </row>
+    <row r="4023" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4023" s="1">
+        <v>44586</v>
+      </c>
+      <c r="B4023" s="21">
+        <v>7.3888882230921278E-3</v>
+      </c>
+      <c r="C4023" s="21">
+        <v>-3.3698663492319784E-3</v>
+      </c>
+      <c r="D4023" s="21">
+        <v>4.0190218738601494E-3</v>
+      </c>
+    </row>
+    <row r="4024" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4024" s="1">
+        <v>44587</v>
+      </c>
+      <c r="B4024" s="21">
+        <v>1.150461249506393E-3</v>
+      </c>
+      <c r="C4024" s="21">
+        <v>-2.6491645466194343E-4</v>
+      </c>
+      <c r="D4024" s="21">
+        <v>8.8554479484444953E-4</v>
+      </c>
+    </row>
+    <row r="4025" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4025" s="1">
+        <v>44588</v>
+      </c>
+      <c r="B4025" s="21">
+        <v>3.6909233634637678E-3</v>
+      </c>
+      <c r="C4025" s="21">
+        <v>1.1848909322092784E-3</v>
+      </c>
+      <c r="D4025" s="21">
+        <v>4.875814295673046E-3</v>
+      </c>
+    </row>
+    <row r="4026" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4026" s="1">
+        <v>44589</v>
+      </c>
+      <c r="B4026" s="21">
+        <v>-1.6819903365913907E-2</v>
+      </c>
+      <c r="C4026" s="21">
+        <v>5.4598684089834388E-3</v>
+      </c>
+      <c r="D4026" s="21">
+        <v>-1.1360034956930469E-2</v>
+      </c>
+    </row>
+    <row r="4027" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4027" s="1">
+        <v>44592</v>
+      </c>
+      <c r="B4027" s="21">
+        <v>-1.1131823636490606E-2</v>
+      </c>
+      <c r="C4027" s="21">
+        <v>4.0312611391692546E-3</v>
+      </c>
+      <c r="D4027" s="21">
+        <v>-7.1005624973213511E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data to 5/31/2022
</commit_message>
<xml_diff>
--- a/EquityHedging/data/update_strats/put_spread_data.xlsx
+++ b/EquityHedging/data/update_strats/put_spread_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20386"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\AC_MNG\Accounts\UPS\Requests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nvg9hxp\Documents\Projects\RMP\EquityHedging\data\update_strats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B39029AB-EFB0-4FFA-B9F8-AF319DC5EFD4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4608C99E-ECCE-4377-8774-09B782E6EA06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1248" yWindow="1248" windowWidth="17280" windowHeight="9108" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="3" r:id="rId1"/>
@@ -28,6 +28,15 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -66,7 +75,7 @@
     <t>Source: Bloomberg, NISA Calculations</t>
   </si>
   <si>
-    <t>As of April 30, 2022</t>
+    <t>As of May 31, 2022</t>
   </si>
 </sst>
 </file>
@@ -1006,7 +1015,7 @@
   </sheetPr>
   <dimension ref="B9:B25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1066,9 +1075,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D199"/>
+  <dimension ref="A1:D200"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A180" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -3857,6 +3866,20 @@
         <v>2.2271900375616882E-2</v>
       </c>
     </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" s="1">
+        <v>44712</v>
+      </c>
+      <c r="B200" s="12">
+        <v>-1.3865026855004237E-2</v>
+      </c>
+      <c r="C200" s="12">
+        <v>1.5905177182930719E-2</v>
+      </c>
+      <c r="D200" s="12">
+        <v>2.0401503279264821E-3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3864,10 +3887,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F4089"/>
+  <dimension ref="A1:F4110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A4072" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A4075" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -61112,6 +61135,300 @@
       </c>
       <c r="D4089" s="21">
         <v>1.3778898286928964E-2</v>
+      </c>
+    </row>
+    <row r="4090" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4090" s="1">
+        <v>44683</v>
+      </c>
+      <c r="B4090" s="21">
+        <v>-4.0226528923929398E-3</v>
+      </c>
+      <c r="C4090" s="21">
+        <v>1.759659360827644E-3</v>
+      </c>
+      <c r="D4090" s="21">
+        <v>-2.2629935315652957E-3</v>
+      </c>
+    </row>
+    <row r="4091" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4091" s="1">
+        <v>44684</v>
+      </c>
+      <c r="B4091" s="21">
+        <v>-3.078996310911073E-3</v>
+      </c>
+      <c r="C4091" s="21">
+        <v>3.3907251658292074E-3</v>
+      </c>
+      <c r="D4091" s="21">
+        <v>3.1172885491813438E-4</v>
+      </c>
+    </row>
+    <row r="4092" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4092" s="1">
+        <v>44685</v>
+      </c>
+      <c r="B4092" s="21">
+        <v>-2.0866558786818326E-2</v>
+      </c>
+      <c r="C4092" s="21">
+        <v>5.4293859804122428E-3</v>
+      </c>
+      <c r="D4092" s="21">
+        <v>-1.5437172806406083E-2</v>
+      </c>
+    </row>
+    <row r="4093" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4093" s="1">
+        <v>44686</v>
+      </c>
+      <c r="B4093" s="21">
+        <v>1.9897881362203194E-2</v>
+      </c>
+      <c r="C4093" s="21">
+        <v>-6.8607183446452872E-3</v>
+      </c>
+      <c r="D4093" s="21">
+        <v>1.3037163017557907E-2</v>
+      </c>
+    </row>
+    <row r="4094" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4094" s="1">
+        <v>44687</v>
+      </c>
+      <c r="B4094" s="21">
+        <v>4.123186010398067E-3</v>
+      </c>
+      <c r="C4094" s="21">
+        <v>-2.384733117239347E-4</v>
+      </c>
+      <c r="D4094" s="21">
+        <v>3.8847126986741322E-3</v>
+      </c>
+    </row>
+    <row r="4095" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4095" s="1">
+        <v>44690</v>
+      </c>
+      <c r="B4095" s="21">
+        <v>2.4546111888950582E-2</v>
+      </c>
+      <c r="C4095" s="21">
+        <v>5.4441267176187055E-8</v>
+      </c>
+      <c r="D4095" s="21">
+        <v>2.4546166330217757E-2</v>
+      </c>
+    </row>
+    <row r="4096" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4096" s="1">
+        <v>44691</v>
+      </c>
+      <c r="B4096" s="21">
+        <v>-2.073202034859307E-3</v>
+      </c>
+      <c r="C4096" s="21">
+        <v>-8.1712488101213232E-3</v>
+      </c>
+      <c r="D4096" s="21">
+        <v>-1.0244450844980629E-2</v>
+      </c>
+    </row>
+    <row r="4097" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4097" s="1">
+        <v>44692</v>
+      </c>
+      <c r="B4097" s="21">
+        <v>1.3202047133750923E-2</v>
+      </c>
+      <c r="C4097" s="21">
+        <v>-3.2989658828231879E-3</v>
+      </c>
+      <c r="D4097" s="21">
+        <v>9.9030812509277345E-3</v>
+      </c>
+    </row>
+    <row r="4098" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4098" s="1">
+        <v>44693</v>
+      </c>
+      <c r="B4098" s="21">
+        <v>6.2405890422280116E-4</v>
+      </c>
+      <c r="C4098" s="21">
+        <v>-2.784420474272545E-3</v>
+      </c>
+      <c r="D4098" s="21">
+        <v>-2.1603615700497439E-3</v>
+      </c>
+    </row>
+    <row r="4099" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4099" s="1">
+        <v>44694</v>
+      </c>
+      <c r="B4099" s="21">
+        <v>-1.9226509912098094E-2</v>
+      </c>
+      <c r="C4099" s="21">
+        <v>1.2473816621318919E-2</v>
+      </c>
+      <c r="D4099" s="21">
+        <v>-6.7526932907791756E-3</v>
+      </c>
+    </row>
+    <row r="4100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4100" s="1">
+        <v>44697</v>
+      </c>
+      <c r="B4100" s="21">
+        <v>3.0496793718251432E-3</v>
+      </c>
+      <c r="C4100" s="21">
+        <v>1.3986870829388997E-3</v>
+      </c>
+      <c r="D4100" s="21">
+        <v>4.4483664547640429E-3</v>
+      </c>
+    </row>
+    <row r="4101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4101" s="1">
+        <v>44698</v>
+      </c>
+      <c r="B4101" s="21">
+        <v>-1.7017216615697318E-2</v>
+      </c>
+      <c r="C4101" s="21">
+        <v>6.6528145592576349E-3</v>
+      </c>
+      <c r="D4101" s="21">
+        <v>-1.0364402056439683E-2</v>
+      </c>
+    </row>
+    <row r="4102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4102" s="1">
+        <v>44699</v>
+      </c>
+      <c r="B4102" s="21">
+        <v>3.4269303665537459E-2</v>
+      </c>
+      <c r="C4102" s="21">
+        <v>-1.4292798694317637E-2</v>
+      </c>
+      <c r="D4102" s="21">
+        <v>1.9976504971219822E-2</v>
+      </c>
+    </row>
+    <row r="4103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4103" s="1">
+        <v>44700</v>
+      </c>
+      <c r="B4103" s="21">
+        <v>5.2078311394811961E-3</v>
+      </c>
+      <c r="C4103" s="21">
+        <v>-3.9129337116130749E-4</v>
+      </c>
+      <c r="D4103" s="21">
+        <v>4.8165377683198887E-3</v>
+      </c>
+    </row>
+    <row r="4104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4104" s="1">
+        <v>44701</v>
+      </c>
+      <c r="B4104" s="21">
+        <v>-3.686788846823236E-4</v>
+      </c>
+      <c r="C4104" s="21">
+        <v>1.9936948445827209E-3</v>
+      </c>
+      <c r="D4104" s="21">
+        <v>1.6250159599003973E-3</v>
+      </c>
+    </row>
+    <row r="4105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4105" s="1">
+        <v>44704</v>
+      </c>
+      <c r="B4105" s="21">
+        <v>-1.5233432007942775E-2</v>
+      </c>
+      <c r="C4105" s="21">
+        <v>9.4137566650262308E-3</v>
+      </c>
+      <c r="D4105" s="21">
+        <v>-5.819675342916544E-3</v>
+      </c>
+    </row>
+    <row r="4106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4106" s="1">
+        <v>44705</v>
+      </c>
+      <c r="B4106" s="21">
+        <v>6.7514689602478197E-3</v>
+      </c>
+      <c r="C4106" s="21">
+        <v>-1.5463206914843178E-3</v>
+      </c>
+      <c r="D4106" s="21">
+        <v>5.2051482687635016E-3</v>
+      </c>
+    </row>
+    <row r="4107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4107" s="1">
+        <v>44706</v>
+      </c>
+      <c r="B4107" s="21">
+        <v>-7.9942262664193867E-3</v>
+      </c>
+      <c r="C4107" s="21">
+        <v>3.3364974450395507E-3</v>
+      </c>
+      <c r="D4107" s="21">
+        <v>-4.6577288213798355E-3</v>
+      </c>
+    </row>
+    <row r="4108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4108" s="1">
+        <v>44707</v>
+      </c>
+      <c r="B4108" s="21">
+        <v>-1.7060801686630128E-2</v>
+      </c>
+      <c r="C4108" s="21">
+        <v>6.1630854520206731E-3</v>
+      </c>
+      <c r="D4108" s="21">
+        <v>-1.0897716234609455E-2</v>
+      </c>
+    </row>
+    <row r="4109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4109" s="1">
+        <v>44708</v>
+      </c>
+      <c r="B4109" s="21">
+        <v>-2.1792753563522557E-2</v>
+      </c>
+      <c r="C4109" s="21">
+        <v>1.5871557251562337E-3</v>
+      </c>
+      <c r="D4109" s="21">
+        <v>-2.0205597838366323E-2</v>
+      </c>
+    </row>
+    <row r="4110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4110" s="1">
+        <v>44712</v>
+      </c>
+      <c r="B4110" s="21">
+        <v>5.4249682774058141E-3</v>
+      </c>
+      <c r="C4110" s="21">
+        <v>1.2978414813451082E-4</v>
+      </c>
+      <c r="D4110" s="21">
+        <v>5.5547524255403248E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update returns data 11/30/22
</commit_message>
<xml_diff>
--- a/EquityHedging/data/update_strats/put_spread_data.xlsx
+++ b/EquityHedging/data/update_strats/put_spread_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RRQ1FYQ\Documents\RMP\EquityHedging\data\update_strats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FCE7FD2E-BB24-4D06-9AA4-F46346837EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{606E3F26-C345-4B1A-83C1-2705C256D084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10305" yWindow="3360" windowWidth="19185" windowHeight="10785" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-60" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="3" r:id="rId1"/>
@@ -75,7 +75,7 @@
     <t>Source: Bloomberg, NISA Calculations</t>
   </si>
   <si>
-    <t>As of October 31, 2022</t>
+    <t>As of November 30, 2022</t>
   </si>
 </sst>
 </file>
@@ -1075,11 +1075,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D205"/>
+  <dimension ref="A1:D206"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A180" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A205" sqref="A205:D205"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3950,6 +3950,20 @@
         <v>-2.9608513570987594E-2</v>
       </c>
     </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A206" s="8">
+        <v>44895</v>
+      </c>
+      <c r="B206" s="7">
+        <v>-2.8814922615576166E-2</v>
+      </c>
+      <c r="C206" s="7">
+        <v>5.0898262604763822E-3</v>
+      </c>
+      <c r="D206" s="7">
+        <v>-2.3725096355099784E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3957,11 +3971,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F4214"/>
+  <dimension ref="A1:F4235"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A4181" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4214" sqref="A4214"/>
+      <pane ySplit="2" topLeftCell="A4199" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4210" sqref="C4210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -62955,6 +62969,300 @@
       </c>
       <c r="D4214" s="21">
         <v>3.3102241662285353E-3</v>
+      </c>
+    </row>
+    <row r="4215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4215" s="1">
+        <v>44866</v>
+      </c>
+      <c r="B4215" s="21">
+        <v>2.3282130651358893E-3</v>
+      </c>
+      <c r="C4215" s="21">
+        <v>-2.2596915582493774E-4</v>
+      </c>
+      <c r="D4215" s="21">
+        <v>2.1022439093109514E-3</v>
+      </c>
+    </row>
+    <row r="4216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4216" s="1">
+        <v>44867</v>
+      </c>
+      <c r="B4216" s="21">
+        <v>1.4108912526755465E-2</v>
+      </c>
+      <c r="C4216" s="21">
+        <v>-3.0368255258989476E-3</v>
+      </c>
+      <c r="D4216" s="21">
+        <v>1.1082324036030886E-2</v>
+      </c>
+    </row>
+    <row r="4217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4217" s="1">
+        <v>44868</v>
+      </c>
+      <c r="B4217" s="21">
+        <v>7.3552589499025446E-3</v>
+      </c>
+      <c r="C4217" s="21">
+        <v>-1.4942503356313425E-3</v>
+      </c>
+      <c r="D4217" s="21">
+        <v>5.9089789453700102E-3</v>
+      </c>
+    </row>
+    <row r="4218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4218" s="1">
+        <v>44869</v>
+      </c>
+      <c r="B4218" s="21">
+        <v>-1.0026020664606811E-2</v>
+      </c>
+      <c r="C4218" s="21">
+        <v>3.2811188601919151E-3</v>
+      </c>
+      <c r="D4218" s="21">
+        <v>-6.8687342346165185E-3</v>
+      </c>
+    </row>
+    <row r="4219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4219" s="1">
+        <v>44872</v>
+      </c>
+      <c r="B4219" s="21">
+        <v>-6.5019875494130358E-3</v>
+      </c>
+      <c r="C4219" s="21">
+        <v>2.411069839376175E-3</v>
+      </c>
+      <c r="D4219" s="21">
+        <v>-4.1330496831556256E-3</v>
+      </c>
+    </row>
+    <row r="4220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4220" s="1">
+        <v>44873</v>
+      </c>
+      <c r="B4220" s="21">
+        <v>-3.4254364559321866E-3</v>
+      </c>
+      <c r="C4220" s="21">
+        <v>8.7779632060201555E-5</v>
+      </c>
+      <c r="D4220" s="21">
+        <v>-3.3351426164046453E-3</v>
+      </c>
+    </row>
+    <row r="4221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4221" s="1">
+        <v>44874</v>
+      </c>
+      <c r="B4221" s="21">
+        <v>1.2925273003474696E-2</v>
+      </c>
+      <c r="C4221" s="21">
+        <v>-2.4177815759468323E-3</v>
+      </c>
+      <c r="D4221" s="21">
+        <v>1.0503264194774512E-2</v>
+      </c>
+    </row>
+    <row r="4222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4222" s="1">
+        <v>44875</v>
+      </c>
+      <c r="B4222" s="21">
+        <v>-3.9659021606061565E-2</v>
+      </c>
+      <c r="C4222" s="21">
+        <v>5.5264807323398678E-3</v>
+      </c>
+      <c r="D4222" s="21">
+        <v>-3.4278086057117851E-2</v>
+      </c>
+    </row>
+    <row r="4223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4223" s="1">
+        <v>44876</v>
+      </c>
+      <c r="B4223" s="21">
+        <v>-4.0015712238116339E-3</v>
+      </c>
+      <c r="C4223" s="21">
+        <v>2.7000129870687121E-4</v>
+      </c>
+      <c r="D4223" s="21">
+        <v>-3.7082748926241743E-3</v>
+      </c>
+    </row>
+    <row r="4224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4224" s="1">
+        <v>44879</v>
+      </c>
+      <c r="B4224" s="21">
+        <v>2.8978725634285596E-3</v>
+      </c>
+      <c r="C4224" s="21">
+        <v>4.9544829280157617E-5</v>
+      </c>
+      <c r="D4224" s="21">
+        <v>2.935826475987691E-3</v>
+      </c>
+    </row>
+    <row r="4225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4225" s="1">
+        <v>44880</v>
+      </c>
+      <c r="B4225" s="21">
+        <v>-3.2585089879413687E-3</v>
+      </c>
+      <c r="C4225" s="21">
+        <v>5.0635411486886074E-5</v>
+      </c>
+      <c r="D4225" s="21">
+        <v>-3.1918609260648692E-3</v>
+      </c>
+    </row>
+    <row r="4226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4226" s="1">
+        <v>44881</v>
+      </c>
+      <c r="B4226" s="21">
+        <v>2.610514628553157E-3</v>
+      </c>
+      <c r="C4226" s="21">
+        <v>1.435337467892821E-4</v>
+      </c>
+      <c r="D4226" s="21">
+        <v>2.7461846038347487E-3</v>
+      </c>
+    </row>
+    <row r="4227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4227" s="1">
+        <v>44882</v>
+      </c>
+      <c r="B4227" s="21">
+        <v>1.2474345307446624E-3</v>
+      </c>
+      <c r="C4227" s="21">
+        <v>5.0437015283860899E-5</v>
+      </c>
+      <c r="D4227" s="21">
+        <v>1.2932912485911063E-3</v>
+      </c>
+    </row>
+    <row r="4228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4228" s="1">
+        <v>44883</v>
+      </c>
+      <c r="B4228" s="21">
+        <v>-1.884021368951505E-3</v>
+      </c>
+      <c r="C4228" s="21">
+        <v>1.380232799357141E-4</v>
+      </c>
+      <c r="D4228" s="21">
+        <v>-1.7336063388197823E-3</v>
+      </c>
+    </row>
+    <row r="4229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4229" s="1">
+        <v>44886</v>
+      </c>
+      <c r="B4229" s="21">
+        <v>1.4078944164772158E-3</v>
+      </c>
+      <c r="C4229" s="21">
+        <v>1.1913345764076814E-4</v>
+      </c>
+      <c r="D4229" s="21">
+        <v>1.5232761736166979E-3</v>
+      </c>
+    </row>
+    <row r="4230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4230" s="1">
+        <v>44887</v>
+      </c>
+      <c r="B4230" s="21">
+        <v>-4.8639653734846742E-3</v>
+      </c>
+      <c r="C4230" s="21">
+        <v>4.5653945295801506E-5</v>
+      </c>
+      <c r="D4230" s="21">
+        <v>-4.7926851751652361E-3</v>
+      </c>
+    </row>
+    <row r="4231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4231" s="1">
+        <v>44888</v>
+      </c>
+      <c r="B4231" s="21">
+        <v>-1.0851919607849903E-3</v>
+      </c>
+      <c r="C4231" s="21">
+        <v>5.148193986894041E-5</v>
+      </c>
+      <c r="D4231" s="21">
+        <v>-1.0266186624881368E-3</v>
+      </c>
+    </row>
+    <row r="4232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4232" s="1">
+        <v>44890</v>
+      </c>
+      <c r="B4232" s="21">
+        <v>1.1522835946257892E-5</v>
+      </c>
+      <c r="C4232" s="21">
+        <v>1.8207057941837519E-5</v>
+      </c>
+      <c r="D4232" s="21">
+        <v>3.0239927983996276E-5</v>
+      </c>
+    </row>
+    <row r="4233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4233" s="1">
+        <v>44893</v>
+      </c>
+      <c r="B4233" s="21">
+        <v>1.2139904054073881E-3</v>
+      </c>
+      <c r="C4233" s="21">
+        <v>1.8451971128355642E-5</v>
+      </c>
+      <c r="D4233" s="21">
+        <v>1.2267303293472598E-3</v>
+      </c>
+    </row>
+    <row r="4234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4234" s="1">
+        <v>44894</v>
+      </c>
+      <c r="B4234" s="21">
+        <v>4.9502128771456713E-4</v>
+      </c>
+      <c r="C4234" s="21">
+        <v>2.2443568173258294E-5</v>
+      </c>
+      <c r="D4234" s="21">
+        <v>5.1556798644916441E-4</v>
+      </c>
+    </row>
+    <row r="4235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4235" s="1">
+        <v>44895</v>
+      </c>
+      <c r="B4235" s="21">
+        <v>0</v>
+      </c>
+      <c r="C4235" s="21">
+        <v>0</v>
+      </c>
+      <c r="D4235" s="21">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update to include new VRR data and pull Vrr2 and trend from vrr_tracks_Data
</commit_message>
<xml_diff>
--- a/EquityHedging/data/update_strats/put_spread_data.xlsx
+++ b/EquityHedging/data/update_strats/put_spread_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RRQ1FYQ\Documents\RMP\EquityHedging\data\update_strats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1ADAF857-26CF-4887-A5EC-1CC1585C3A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1EA4BEC6-DCC0-4A80-B0BC-40FE0165859A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57710" yWindow="-110" windowWidth="29020" windowHeight="15820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
     <definedName name="solver_typ" hidden="1">3</definedName>
     <definedName name="solver_val" hidden="1">0</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029" iterate="1" iterateCount="1000"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -75,7 +75,7 @@
     <t>Source: Bloomberg, NISA Calculations</t>
   </si>
   <si>
-    <t>As of December 31, 2022</t>
+    <t>As of January 31, 2023</t>
   </si>
 </sst>
 </file>
@@ -1019,7 +1019,9 @@
   </sheetPr>
   <dimension ref="B9:B25"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1079,7 +1081,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D207"/>
+  <dimension ref="A1:D208"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A184" activePane="bottomLeft" state="frozen"/>
@@ -3982,6 +3984,20 @@
         <v>2.3940257310590907E-2</v>
       </c>
     </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A208" s="8">
+        <v>44957</v>
+      </c>
+      <c r="B208" s="7">
+        <v>-3.9321216872663656E-2</v>
+      </c>
+      <c r="C208" s="7">
+        <v>1.4397693826237123E-2</v>
+      </c>
+      <c r="D208" s="7">
+        <v>-2.4923523046426754E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3989,11 +4005,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F4256"/>
+  <dimension ref="A1:F4276"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A4233" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="2" topLeftCell="A4254" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E4284" sqref="E4284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -63575,6 +63591,286 @@
       </c>
       <c r="D4256" s="21">
         <v>1.9000748078276529E-3</v>
+      </c>
+    </row>
+    <row r="4257" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4257" s="1">
+        <v>44929</v>
+      </c>
+      <c r="B4257" s="21">
+        <v>2.587424332463323E-3</v>
+      </c>
+      <c r="C4257" s="21">
+        <v>-8.1006023664443867E-4</v>
+      </c>
+      <c r="D4257" s="21">
+        <v>1.7773640958188845E-3</v>
+      </c>
+    </row>
+    <row r="4258" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4258" s="1">
+        <v>44930</v>
+      </c>
+      <c r="B4258" s="21">
+        <v>-5.1384632407951488E-3</v>
+      </c>
+      <c r="C4258" s="21">
+        <v>2.8606883596469157E-3</v>
+      </c>
+      <c r="D4258" s="21">
+        <v>-2.2893186430983834E-3</v>
+      </c>
+    </row>
+    <row r="4259" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4259" s="1">
+        <v>44931</v>
+      </c>
+      <c r="B4259" s="21">
+        <v>7.9561951339550997E-3</v>
+      </c>
+      <c r="C4259" s="21">
+        <v>-2.0972198611025872E-3</v>
+      </c>
+      <c r="D4259" s="21">
+        <v>5.8372893492312046E-3</v>
+      </c>
+    </row>
+    <row r="4260" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4260" s="1">
+        <v>44932</v>
+      </c>
+      <c r="B4260" s="21">
+        <v>-1.6094581162025435E-2</v>
+      </c>
+      <c r="C4260" s="21">
+        <v>5.4858996520733136E-3</v>
+      </c>
+      <c r="D4260" s="21">
+        <v>-1.0638844686219156E-2</v>
+      </c>
+    </row>
+    <row r="4261" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4261" s="1">
+        <v>44935</v>
+      </c>
+      <c r="B4261" s="21">
+        <v>2.8963943935094306E-4</v>
+      </c>
+      <c r="C4261" s="21">
+        <v>3.6365010729900287E-5</v>
+      </c>
+      <c r="D4261" s="21">
+        <v>3.2481772096663723E-4</v>
+      </c>
+    </row>
+    <row r="4262" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4262" s="1">
+        <v>44936</v>
+      </c>
+      <c r="B4262" s="21">
+        <v>-4.4761184931036372E-3</v>
+      </c>
+      <c r="C4262" s="21">
+        <v>2.2819070734965436E-3</v>
+      </c>
+      <c r="D4262" s="21">
+        <v>-2.1454726940062243E-3</v>
+      </c>
+    </row>
+    <row r="4263" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4263" s="1">
+        <v>44937</v>
+      </c>
+      <c r="B4263" s="21">
+        <v>-7.8357505090226268E-3</v>
+      </c>
+      <c r="C4263" s="21">
+        <v>1.5525183386074851E-3</v>
+      </c>
+      <c r="D4263" s="21">
+        <v>-6.1985785463491141E-3</v>
+      </c>
+    </row>
+    <row r="4264" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4264" s="1">
+        <v>44938</v>
+      </c>
+      <c r="B4264" s="21">
+        <v>-1.9053213192155127E-3</v>
+      </c>
+      <c r="C4264" s="21">
+        <v>1.8197444846472714E-3</v>
+      </c>
+      <c r="D4264" s="21">
+        <v>-2.5751074426895515E-5</v>
+      </c>
+    </row>
+    <row r="4265" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4265" s="1">
+        <v>44939</v>
+      </c>
+      <c r="B4265" s="21">
+        <v>-2.0588276773801876E-3</v>
+      </c>
+      <c r="C4265" s="21">
+        <v>6.7548563055054285E-4</v>
+      </c>
+      <c r="D4265" s="21">
+        <v>-1.343248442533404E-3</v>
+      </c>
+    </row>
+    <row r="4266" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4266" s="1">
+        <v>44943</v>
+      </c>
+      <c r="B4266" s="21">
+        <v>1.1721920119559884E-3</v>
+      </c>
+      <c r="C4266" s="21">
+        <v>-1.6041913518399023E-5</v>
+      </c>
+      <c r="D4266" s="21">
+        <v>1.1416231334650073E-3</v>
+      </c>
+    </row>
+    <row r="4267" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4267" s="1">
+        <v>44944</v>
+      </c>
+      <c r="B4267" s="21">
+        <v>8.8409592731717532E-3</v>
+      </c>
+      <c r="C4267" s="21">
+        <v>-1.7110638254414492E-3</v>
+      </c>
+      <c r="D4267" s="21">
+        <v>6.9797964758550081E-3</v>
+      </c>
+    </row>
+    <row r="4268" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4268" s="1">
+        <v>44945</v>
+      </c>
+      <c r="B4268" s="21">
+        <v>4.9880619195996076E-3</v>
+      </c>
+      <c r="C4268" s="21">
+        <v>-9.0729819786303299E-4</v>
+      </c>
+      <c r="D4268" s="21">
+        <v>4.0147144467576308E-3</v>
+      </c>
+    </row>
+    <row r="4269" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4269" s="1">
+        <v>44946</v>
+      </c>
+      <c r="B4269" s="21">
+        <v>-1.2860068156421807E-2</v>
+      </c>
+      <c r="C4269" s="21">
+        <v>2.4294934200936205E-3</v>
+      </c>
+      <c r="D4269" s="21">
+        <v>-1.0283214256134184E-2</v>
+      </c>
+    </row>
+    <row r="4270" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4270" s="1">
+        <v>44949</v>
+      </c>
+      <c r="B4270" s="21">
+        <v>-7.1264879945913953E-3</v>
+      </c>
+      <c r="C4270" s="21">
+        <v>1.1608005365431838E-3</v>
+      </c>
+      <c r="D4270" s="21">
+        <v>-5.8527647990220351E-3</v>
+      </c>
+    </row>
+    <row r="4271" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4271" s="1">
+        <v>44950</v>
+      </c>
+      <c r="B4271" s="21">
+        <v>4.7816269551759325E-4</v>
+      </c>
+      <c r="C4271" s="21">
+        <v>3.9622841402567961E-4</v>
+      </c>
+      <c r="D4271" s="21">
+        <v>8.8088374361501641E-4</v>
+      </c>
+    </row>
+    <row r="4272" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4272" s="1">
+        <v>44951</v>
+      </c>
+      <c r="B4272" s="21">
+        <v>9.5176887363067667E-5</v>
+      </c>
+      <c r="C4272" s="21">
+        <v>6.3001713729973779E-5</v>
+      </c>
+      <c r="D4272" s="21">
+        <v>1.5889171467718872E-4</v>
+      </c>
+    </row>
+    <row r="4273" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4273" s="1">
+        <v>44952</v>
+      </c>
+      <c r="B4273" s="21">
+        <v>-5.7099352584341389E-3</v>
+      </c>
+      <c r="C4273" s="21">
+        <v>6.731430097905351E-4</v>
+      </c>
+      <c r="D4273" s="21">
+        <v>-4.9383952549871104E-3</v>
+      </c>
+    </row>
+    <row r="4274" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4274" s="1">
+        <v>44953</v>
+      </c>
+      <c r="B4274" s="21">
+        <v>-9.9105752748285042E-4</v>
+      </c>
+      <c r="C4274" s="21">
+        <v>3.0170697791386518E-4</v>
+      </c>
+      <c r="D4274" s="21">
+        <v>-6.639278548363158E-4</v>
+      </c>
+    </row>
+    <row r="4275" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4275" s="1">
+        <v>44956</v>
+      </c>
+      <c r="B4275" s="21">
+        <v>5.4568110042226966E-3</v>
+      </c>
+      <c r="C4275" s="21">
+        <v>-5.1598968259745795E-4</v>
+      </c>
+      <c r="D4275" s="21">
+        <v>4.841348402305364E-3</v>
+      </c>
+    </row>
+    <row r="4276" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4276" s="1">
+        <v>44957</v>
+      </c>
+      <c r="B4276" s="21">
+        <v>-7.3395675001654845E-3</v>
+      </c>
+      <c r="C4276" s="21">
+        <v>6.4920894504354437E-4</v>
+      </c>
+      <c r="D4276" s="21">
+        <v>-6.5663075172980164E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update putspread and vrrtracks
</commit_message>
<xml_diff>
--- a/EquityHedging/data/update_strats/put_spread_data.xlsx
+++ b/EquityHedging/data/update_strats/put_spread_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RRQ1FYQ\Documents\RMP\EquityHedging\data\update_strats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\AC_MNG\Accounts\UPS\Presentations\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{069FC8E3-7F39-49D6-A4A9-6C5831EB9EFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D62448E-692F-4CCD-B4D9-099AE5C8BA65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="3" r:id="rId1"/>
@@ -75,7 +75,7 @@
     <t>Source: Bloomberg, NISA Calculations</t>
   </si>
   <si>
-    <t>As of February 28, 2023</t>
+    <t>As of March 31, 2023</t>
   </si>
 </sst>
 </file>
@@ -1019,7 +1019,7 @@
   </sheetPr>
   <dimension ref="B9:B25"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1079,7 +1079,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D209"/>
+  <dimension ref="A1:D210"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A184" activePane="bottomLeft" state="frozen"/>
@@ -4010,6 +4010,20 @@
         <v>8.70102412756113E-3</v>
       </c>
     </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A210" s="8">
+        <v>45016</v>
+      </c>
+      <c r="B210" s="7">
+        <v>-1.3167376351812754E-2</v>
+      </c>
+      <c r="C210" s="7">
+        <v>8.3073351758704561E-3</v>
+      </c>
+      <c r="D210" s="7">
+        <v>-4.860041175942742E-3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4017,10 +4031,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F4295"/>
+  <dimension ref="A1:F4318"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A4263" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A4279" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -64149,6 +64163,328 @@
       </c>
       <c r="D4295" s="21">
         <v>3.04646878601181E-3</v>
+      </c>
+    </row>
+    <row r="4296" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4296" s="1">
+        <v>44986</v>
+      </c>
+      <c r="B4296" s="21">
+        <v>1.9551849140096106E-3</v>
+      </c>
+      <c r="C4296" s="23">
+        <v>-1.5678249188974392E-4</v>
+      </c>
+      <c r="D4296" s="21">
+        <v>1.7984024221198668E-3</v>
+      </c>
+    </row>
+    <row r="4297" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4297" s="1">
+        <v>44987</v>
+      </c>
+      <c r="B4297" s="21">
+        <v>-2.8384272453391784E-3</v>
+      </c>
+      <c r="C4297" s="23">
+        <v>1.7008205881268341E-3</v>
+      </c>
+      <c r="D4297" s="21">
+        <v>-1.141370323078449E-3</v>
+      </c>
+    </row>
+    <row r="4298" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4298" s="1">
+        <v>44988</v>
+      </c>
+      <c r="B4298" s="21">
+        <v>-6.7118701423551563E-3</v>
+      </c>
+      <c r="C4298" s="23">
+        <v>3.0835586145996278E-3</v>
+      </c>
+      <c r="D4298" s="21">
+        <v>-3.6152178682455445E-3</v>
+      </c>
+    </row>
+    <row r="4299" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4299" s="1">
+        <v>44991</v>
+      </c>
+      <c r="B4299" s="21">
+        <v>-3.027128276493423E-4</v>
+      </c>
+      <c r="C4299" s="23">
+        <v>4.9356311662346602E-4</v>
+      </c>
+      <c r="D4299" s="21">
+        <v>1.9601624900819891E-4</v>
+      </c>
+    </row>
+    <row r="4300" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4300" s="1">
+        <v>44992</v>
+      </c>
+      <c r="B4300" s="21">
+        <v>6.3296896581928287E-3</v>
+      </c>
+      <c r="C4300" s="23">
+        <v>-2.1834120044306048E-3</v>
+      </c>
+      <c r="D4300" s="21">
+        <v>4.0964432074009904E-3</v>
+      </c>
+    </row>
+    <row r="4301" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4301" s="1">
+        <v>44993</v>
+      </c>
+      <c r="B4301" s="21">
+        <v>-5.8084850902545993E-4</v>
+      </c>
+      <c r="C4301" s="23">
+        <v>8.1745522843407322E-4</v>
+      </c>
+      <c r="D4301" s="21">
+        <v>2.3962707250250765E-4</v>
+      </c>
+    </row>
+    <row r="4302" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4302" s="1">
+        <v>44994</v>
+      </c>
+      <c r="B4302" s="21">
+        <v>7.6533564627513694E-3</v>
+      </c>
+      <c r="C4302" s="23">
+        <v>-5.6963469258165299E-3</v>
+      </c>
+      <c r="D4302" s="21">
+        <v>1.9158439930707005E-3</v>
+      </c>
+    </row>
+    <row r="4303" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4303" s="1">
+        <v>44995</v>
+      </c>
+      <c r="B4303" s="21">
+        <v>5.9994341292295122E-3</v>
+      </c>
+      <c r="C4303" s="23">
+        <v>-3.2986145611378342E-3</v>
+      </c>
+      <c r="D4303" s="21">
+        <v>2.7304512751832066E-3</v>
+      </c>
+    </row>
+    <row r="4304" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4304" s="1">
+        <v>44998</v>
+      </c>
+      <c r="B4304" s="21">
+        <v>8.6208532331045291E-4</v>
+      </c>
+      <c r="C4304" s="23">
+        <v>-2.6424408519433186E-3</v>
+      </c>
+      <c r="D4304" s="21">
+        <v>-1.7457215395740183E-3</v>
+      </c>
+    </row>
+    <row r="4305" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4305" s="1">
+        <v>44999</v>
+      </c>
+      <c r="B4305" s="21">
+        <v>-6.6499772189505379E-3</v>
+      </c>
+      <c r="C4305" s="23">
+        <v>5.5341263322050849E-3</v>
+      </c>
+      <c r="D4305" s="21">
+        <v>-1.2360717487636935E-3</v>
+      </c>
+    </row>
+    <row r="4306" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4306" s="1">
+        <v>45000</v>
+      </c>
+      <c r="B4306" s="21">
+        <v>2.988444462731193E-3</v>
+      </c>
+      <c r="C4306" s="23">
+        <v>-3.8736717340480966E-3</v>
+      </c>
+      <c r="D4306" s="21">
+        <v>-8.5641962827101787E-4</v>
+      </c>
+    </row>
+    <row r="4307" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4307" s="1">
+        <v>45001</v>
+      </c>
+      <c r="B4307" s="21">
+        <v>-7.1623508317348802E-3</v>
+      </c>
+      <c r="C4307" s="23">
+        <v>6.0363664658840965E-3</v>
+      </c>
+      <c r="D4307" s="21">
+        <v>-1.2226106341768578E-3</v>
+      </c>
+    </row>
+    <row r="4308" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4308" s="1">
+        <v>45002</v>
+      </c>
+      <c r="B4308" s="21">
+        <v>4.8543275463737295E-3</v>
+      </c>
+      <c r="C4308" s="23">
+        <v>-5.0370185122925442E-3</v>
+      </c>
+      <c r="D4308" s="21">
+        <v>-1.7441208224019646E-4</v>
+      </c>
+    </row>
+    <row r="4309" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4309" s="1">
+        <v>45005</v>
+      </c>
+      <c r="B4309" s="21">
+        <v>-3.7375795481497651E-3</v>
+      </c>
+      <c r="C4309" s="23">
+        <v>3.7370939963780208E-3</v>
+      </c>
+      <c r="D4309" s="21">
+        <v>-4.3616629741512379E-5</v>
+      </c>
+    </row>
+    <row r="4310" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4310" s="1">
+        <v>45006</v>
+      </c>
+      <c r="B4310" s="21">
+        <v>-5.4098429246428282E-3</v>
+      </c>
+      <c r="C4310" s="23">
+        <v>4.3226837143974465E-3</v>
+      </c>
+      <c r="D4310" s="21">
+        <v>-1.1064663989269466E-3</v>
+      </c>
+    </row>
+    <row r="4311" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4311" s="1">
+        <v>45007</v>
+      </c>
+      <c r="B4311" s="21">
+        <v>6.6526196445140422E-3</v>
+      </c>
+      <c r="C4311" s="23">
+        <v>-3.098935213940441E-3</v>
+      </c>
+      <c r="D4311" s="21">
+        <v>3.5263953580621371E-3</v>
+      </c>
+    </row>
+    <row r="4312" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4312" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B4312" s="21">
+        <v>-7.6612527681676188E-4</v>
+      </c>
+      <c r="C4312" s="23">
+        <v>7.9365580611696603E-4</v>
+      </c>
+      <c r="D4312" s="21">
+        <v>2.431743816704457E-5</v>
+      </c>
+    </row>
+    <row r="4313" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4313" s="1">
+        <v>45009</v>
+      </c>
+      <c r="B4313" s="21">
+        <v>-2.3492859905559476E-3</v>
+      </c>
+      <c r="C4313" s="23">
+        <v>1.5187100334979446E-3</v>
+      </c>
+      <c r="D4313" s="21">
+        <v>-8.340289019925501E-4</v>
+      </c>
+    </row>
+    <row r="4314" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4314" s="1">
+        <v>45012</v>
+      </c>
+      <c r="B4314" s="21">
+        <v>-6.0506181293500149E-4</v>
+      </c>
+      <c r="C4314" s="23">
+        <v>1.6684464206981285E-3</v>
+      </c>
+      <c r="D4314" s="21">
+        <v>1.0635929357065276E-3</v>
+      </c>
+    </row>
+    <row r="4315" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4315" s="1">
+        <v>45013</v>
+      </c>
+      <c r="B4315" s="21">
+        <v>5.7783147747594876E-4</v>
+      </c>
+      <c r="C4315" s="23">
+        <v>5.1308363761754829E-4</v>
+      </c>
+      <c r="D4315" s="21">
+        <v>1.0888477826629245E-3</v>
+      </c>
+    </row>
+    <row r="4316" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4316" s="1">
+        <v>45014</v>
+      </c>
+      <c r="B4316" s="21">
+        <v>-5.6326327342629198E-3</v>
+      </c>
+      <c r="C4316" s="23">
+        <v>2.1168674145266185E-3</v>
+      </c>
+      <c r="D4316" s="21">
+        <v>-3.4937796491093043E-3</v>
+      </c>
+    </row>
+    <row r="4317" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4317" s="1">
+        <v>45015</v>
+      </c>
+      <c r="B4317" s="21">
+        <v>-2.2919821862864807E-3</v>
+      </c>
+      <c r="C4317" s="23">
+        <v>8.3279883857862889E-4</v>
+      </c>
+      <c r="D4317" s="21">
+        <v>-1.4406359073553265E-3</v>
+      </c>
+    </row>
+    <row r="4318" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4318" s="1">
+        <v>45016</v>
+      </c>
+      <c r="B4318" s="21">
+        <v>-5.8459246984677799E-3</v>
+      </c>
+      <c r="C4318" s="23">
+        <v>1.2063379385082069E-3</v>
+      </c>
+      <c r="D4318" s="21">
+        <v>-4.5892271003205335E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vrr and put spread data update
</commit_message>
<xml_diff>
--- a/EquityHedging/data/update_strats/put_spread_data.xlsx
+++ b/EquityHedging/data/update_strats/put_spread_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RRQ1FYQ\Documents\RMP\EquityHedging\data\update_strats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nisa.local\nisa\Client\AC_MNG\Accounts\UPS\Presentations\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC708601-D784-4BA1-86A9-F690E07AA330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74424CDD-DCEA-48BF-9D2D-2EE066FA0D56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="3" r:id="rId1"/>
@@ -75,7 +75,7 @@
     <t>Source: Bloomberg, NISA Calculations</t>
   </si>
   <si>
-    <t>As of May 31, 2023</t>
+    <t>As of June 30, 2023</t>
   </si>
 </sst>
 </file>
@@ -178,7 +178,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -233,6 +233,12 @@
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1079,7 +1085,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D212"/>
+  <dimension ref="A1:D213"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A184" activePane="bottomLeft" state="frozen"/>
@@ -4052,6 +4058,20 @@
         <v>-1.1382391362454447E-3</v>
       </c>
     </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A213" s="8">
+        <v>45107</v>
+      </c>
+      <c r="B213" s="7">
+        <v>-2.2418475489018541E-2</v>
+      </c>
+      <c r="C213" s="7">
+        <v>5.8024350296412841E-3</v>
+      </c>
+      <c r="D213" s="7">
+        <v>-1.6616040459376813E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4059,10 +4079,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F4360"/>
+  <dimension ref="A1:F4381"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A4323" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A4360" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -65090,7 +65110,301 @@
       </c>
     </row>
     <row r="4360" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4360" s="1"/>
+      <c r="A4360" s="1">
+        <v>45078</v>
+      </c>
+      <c r="B4360" s="24">
+        <v>-3.4529248451430701E-3</v>
+      </c>
+      <c r="C4360" s="25">
+        <v>1.6531641278126918E-3</v>
+      </c>
+      <c r="D4360" s="24">
+        <v>-1.7997607173303783E-3</v>
+      </c>
+    </row>
+    <row r="4361" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4361" s="1">
+        <v>45079</v>
+      </c>
+      <c r="B4361" s="24">
+        <v>-5.5515811331628556E-3</v>
+      </c>
+      <c r="C4361" s="25">
+        <v>1.1120547396191677E-3</v>
+      </c>
+      <c r="D4361" s="24">
+        <v>-4.4264854066662128E-3</v>
+      </c>
+    </row>
+    <row r="4362" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4362" s="1">
+        <v>45082</v>
+      </c>
+      <c r="B4362" s="24">
+        <v>6.355283425254801E-4</v>
+      </c>
+      <c r="C4362" s="25">
+        <v>1.8579621976923336E-4</v>
+      </c>
+      <c r="D4362" s="24">
+        <v>8.2123490305208635E-4</v>
+      </c>
+    </row>
+    <row r="4363" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4363" s="1">
+        <v>45083</v>
+      </c>
+      <c r="B4363" s="24">
+        <v>-8.0912118350120793E-4</v>
+      </c>
+      <c r="C4363" s="25">
+        <v>6.4110459667188191E-4</v>
+      </c>
+      <c r="D4363" s="24">
+        <v>-1.6022811849205137E-4</v>
+      </c>
+    </row>
+    <row r="4364" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4364" s="1">
+        <v>45084</v>
+      </c>
+      <c r="B4364" s="24">
+        <v>1.406382588319161E-3</v>
+      </c>
+      <c r="C4364" s="25">
+        <v>-1.3151181150354875E-4</v>
+      </c>
+      <c r="D4364" s="24">
+        <v>1.2685735192283303E-3</v>
+      </c>
+    </row>
+    <row r="4365" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4365" s="1">
+        <v>45085</v>
+      </c>
+      <c r="B4365" s="24">
+        <v>-2.1813051732923958E-3</v>
+      </c>
+      <c r="C4365" s="25">
+        <v>3.7996341225218354E-4</v>
+      </c>
+      <c r="D4365" s="24">
+        <v>-1.7907893348757253E-3</v>
+      </c>
+    </row>
+    <row r="4366" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4366" s="1">
+        <v>45086</v>
+      </c>
+      <c r="B4366" s="24">
+        <v>-6.2528821836801854E-4</v>
+      </c>
+      <c r="C4366" s="25">
+        <v>1.9686639474369624E-5</v>
+      </c>
+      <c r="D4366" s="24">
+        <v>-6.0298555551788571E-4</v>
+      </c>
+    </row>
+    <row r="4367" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4367" s="1">
+        <v>45089</v>
+      </c>
+      <c r="B4367" s="24">
+        <v>-3.4444006813017891E-3</v>
+      </c>
+      <c r="C4367" s="25">
+        <v>2.1430285746588455E-4</v>
+      </c>
+      <c r="D4367" s="24">
+        <v>-3.214418554221866E-3</v>
+      </c>
+    </row>
+    <row r="4368" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4368" s="1">
+        <v>45090</v>
+      </c>
+      <c r="B4368" s="24">
+        <v>-2.5626368979258206E-3</v>
+      </c>
+      <c r="C4368" s="25">
+        <v>2.4407863675597876E-4</v>
+      </c>
+      <c r="D4368" s="24">
+        <v>-2.30455667632829E-3</v>
+      </c>
+    </row>
+    <row r="4369" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4369" s="1">
+        <v>45091</v>
+      </c>
+      <c r="B4369" s="24">
+        <v>-1.5712162213886934E-4</v>
+      </c>
+      <c r="C4369" s="25">
+        <v>2.9686594538194194E-4</v>
+      </c>
+      <c r="D4369" s="24">
+        <v>1.4538572881294675E-4</v>
+      </c>
+    </row>
+    <row r="4370" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4370" s="1">
+        <v>45092</v>
+      </c>
+      <c r="B4370" s="24">
+        <v>-4.676011664833341E-3</v>
+      </c>
+      <c r="C4370" s="25">
+        <v>8.4291812026697616E-5</v>
+      </c>
+      <c r="D4370" s="24">
+        <v>-4.5684166675036501E-3</v>
+      </c>
+    </row>
+    <row r="4371" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4371" s="1">
+        <v>45093</v>
+      </c>
+      <c r="B4371" s="24">
+        <v>1.6127447620554694E-3</v>
+      </c>
+      <c r="C4371" s="25">
+        <v>2.6130266089780538E-4</v>
+      </c>
+      <c r="D4371" s="24">
+        <v>1.8719684147573044E-3</v>
+      </c>
+    </row>
+    <row r="4372" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4372" s="1">
+        <v>45097</v>
+      </c>
+      <c r="B4372" s="24">
+        <v>1.6824283140494331E-3</v>
+      </c>
+      <c r="C4372" s="25">
+        <v>-1.0684086546004713E-4</v>
+      </c>
+      <c r="D4372" s="24">
+        <v>1.5649679779407588E-3</v>
+      </c>
+    </row>
+    <row r="4373" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4373" s="1">
+        <v>45098</v>
+      </c>
+      <c r="B4373" s="24">
+        <v>2.3256071930419747E-3</v>
+      </c>
+      <c r="C4373" s="25">
+        <v>1.2527339051596081E-4</v>
+      </c>
+      <c r="D4373" s="24">
+        <v>2.4417049868759363E-3</v>
+      </c>
+    </row>
+    <row r="4374" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4374" s="1">
+        <v>45099</v>
+      </c>
+      <c r="B4374" s="24">
+        <v>-1.2907552620005003E-3</v>
+      </c>
+      <c r="C4374" s="25">
+        <v>2.9147142430891343E-4</v>
+      </c>
+      <c r="D4374" s="24">
+        <v>-9.8814091916263813E-4</v>
+      </c>
+    </row>
+    <row r="4375" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4375" s="1">
+        <v>45100</v>
+      </c>
+      <c r="B4375" s="24">
+        <v>3.1253553651964978E-3</v>
+      </c>
+      <c r="C4375" s="25">
+        <v>-2.7412922053453732E-4</v>
+      </c>
+      <c r="D4375" s="24">
+        <v>2.8298071564375935E-3</v>
+      </c>
+    </row>
+    <row r="4376" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4376" s="1">
+        <v>45103</v>
+      </c>
+      <c r="B4376" s="24">
+        <v>1.6886766175825932E-3</v>
+      </c>
+      <c r="C4376" s="25">
+        <v>-1.6448108932226069E-5</v>
+      </c>
+      <c r="D4376" s="24">
+        <v>1.6634664443736765E-3</v>
+      </c>
+    </row>
+    <row r="4377" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4377" s="1">
+        <v>45104</v>
+      </c>
+      <c r="B4377" s="24">
+        <v>-4.2584445580055421E-3</v>
+      </c>
+      <c r="C4377" s="25">
+        <v>4.2168201672155854E-4</v>
+      </c>
+      <c r="D4377" s="24">
+        <v>-3.8101495945725926E-3</v>
+      </c>
+    </row>
+    <row r="4378" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4378" s="1">
+        <v>45105</v>
+      </c>
+      <c r="B4378" s="24">
+        <v>1.1162211639184837E-4</v>
+      </c>
+      <c r="C4378" s="25">
+        <v>2.3743048818866501E-4</v>
+      </c>
+      <c r="D4378" s="24">
+        <v>3.5239406382956058E-4</v>
+      </c>
+    </row>
+    <row r="4379" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4379" s="1">
+        <v>45106</v>
+      </c>
+      <c r="B4379" s="24">
+        <v>-1.5606035244983714E-3</v>
+      </c>
+      <c r="C4379" s="25">
+        <v>3.2228635552411287E-5</v>
+      </c>
+      <c r="D4379" s="24">
+        <v>-1.5189249011999034E-3</v>
+      </c>
+    </row>
+    <row r="4380" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4380" s="1">
+        <v>45107</v>
+      </c>
+      <c r="B4380" s="24">
+        <v>-4.6124553687082173E-3</v>
+      </c>
+      <c r="C4380" s="25">
+        <v>1.165372752103655E-4</v>
+      </c>
+      <c r="D4380" s="24">
+        <v>-4.4672608059229818E-3</v>
+      </c>
+    </row>
+    <row r="4381" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4381" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update returns data 6/30/23
</commit_message>
<xml_diff>
--- a/EquityHedging/data/update_strats/put_spread_data.xlsx
+++ b/EquityHedging/data/update_strats/put_spread_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RRQ1FYQ\Documents\RMP\EquityHedging\data\update_strats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F4D0639-26F8-413F-B6F8-FDA57CF6FAAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D686461-A922-464F-B944-F6E06895B56F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="2250" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57710" yWindow="-110" windowWidth="29020" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="3" r:id="rId1"/>
@@ -75,7 +75,7 @@
     <t>Source: Bloomberg, NISA Calculations</t>
   </si>
   <si>
-    <t>As of April 30, 2023</t>
+    <t>As of June 30, 2023</t>
   </si>
 </sst>
 </file>
@@ -178,7 +178,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -233,6 +233,12 @@
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1079,11 +1085,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D211"/>
+  <dimension ref="A1:D213"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A184" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A211" sqref="A211"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4038,6 +4044,34 @@
         <v>-7.0013106546495951E-4</v>
       </c>
     </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A212" s="8">
+        <v>45077</v>
+      </c>
+      <c r="B212" s="7">
+        <v>-2.1742339346643158E-3</v>
+      </c>
+      <c r="C212" s="7">
+        <v>1.0359947984193152E-3</v>
+      </c>
+      <c r="D212" s="7">
+        <v>-1.1382391362454447E-3</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A213" s="8">
+        <v>45107</v>
+      </c>
+      <c r="B213" s="7">
+        <v>-2.2418475489018541E-2</v>
+      </c>
+      <c r="C213" s="7">
+        <v>5.8024350296412841E-3</v>
+      </c>
+      <c r="D213" s="7">
+        <v>-1.6616040459376813E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4045,11 +4079,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F4337"/>
+  <dimension ref="A1:F4381"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A4309" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4337" sqref="A4337"/>
+      <pane ySplit="2" topLeftCell="A4360" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -64766,6 +64800,611 @@
       <c r="D4337" s="21">
         <v>-2.8401810127393181E-3</v>
       </c>
+    </row>
+    <row r="4338" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4338" s="1">
+        <v>45047</v>
+      </c>
+      <c r="B4338" s="21">
+        <v>2.553960562255486E-4</v>
+      </c>
+      <c r="C4338" s="23">
+        <v>-1.926689803120085E-5</v>
+      </c>
+      <c r="D4338" s="21">
+        <v>2.3612915819434775E-4</v>
+      </c>
+    </row>
+    <row r="4339" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4339" s="1">
+        <v>45048</v>
+      </c>
+      <c r="B4339" s="21">
+        <v>4.7486348650108475E-3</v>
+      </c>
+      <c r="C4339" s="23">
+        <v>-4.2016628799237694E-4</v>
+      </c>
+      <c r="D4339" s="21">
+        <v>4.3286673303636544E-3</v>
+      </c>
+    </row>
+    <row r="4340" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4340" s="1">
+        <v>45049</v>
+      </c>
+      <c r="B4340" s="21">
+        <v>2.8573037015260927E-3</v>
+      </c>
+      <c r="C4340" s="23">
+        <v>-8.8025255438341172E-5</v>
+      </c>
+      <c r="D4340" s="21">
+        <v>2.7709668957267893E-3</v>
+      </c>
+    </row>
+    <row r="4341" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4341" s="1">
+        <v>45050</v>
+      </c>
+      <c r="B4341" s="21">
+        <v>2.9495077265187541E-3</v>
+      </c>
+      <c r="C4341" s="23">
+        <v>-6.871228184305877E-4</v>
+      </c>
+      <c r="D4341" s="21">
+        <v>2.2693020384765461E-3</v>
+      </c>
+    </row>
+    <row r="4342" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4342" s="1">
+        <v>45051</v>
+      </c>
+      <c r="B4342" s="21">
+        <v>-7.4539082677605251E-3</v>
+      </c>
+      <c r="C4342" s="23">
+        <v>1.3029968734906954E-3</v>
+      </c>
+      <c r="D4342" s="21">
+        <v>-6.1738774155756281E-3</v>
+      </c>
+    </row>
+    <row r="4343" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4343" s="1">
+        <v>45054</v>
+      </c>
+      <c r="B4343" s="21">
+        <v>-2.3606074715439818E-4</v>
+      </c>
+      <c r="C4343" s="23">
+        <v>2.5226518509636857E-4</v>
+      </c>
+      <c r="D4343" s="21">
+        <v>1.5391586892434871E-5</v>
+      </c>
+    </row>
+    <row r="4344" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4344" s="1">
+        <v>45055</v>
+      </c>
+      <c r="B4344" s="21">
+        <v>1.729260295182096E-3</v>
+      </c>
+      <c r="C4344" s="23">
+        <v>-5.0831198038318202E-5</v>
+      </c>
+      <c r="D4344" s="21">
+        <v>1.6779998850744847E-3</v>
+      </c>
+    </row>
+    <row r="4345" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4345" s="1">
+        <v>45056</v>
+      </c>
+      <c r="B4345" s="21">
+        <v>-1.6476612254815134E-3</v>
+      </c>
+      <c r="C4345" s="23">
+        <v>1.6042739948666777E-4</v>
+      </c>
+      <c r="D4345" s="21">
+        <v>-1.487528737058633E-3</v>
+      </c>
+    </row>
+    <row r="4346" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4346" s="1">
+        <v>45057</v>
+      </c>
+      <c r="B4346" s="21">
+        <v>7.3158891907633102E-4</v>
+      </c>
+      <c r="C4346" s="23">
+        <v>3.813790210104407E-5</v>
+      </c>
+      <c r="D4346" s="21">
+        <v>7.6927943777817796E-4</v>
+      </c>
+    </row>
+    <row r="4347" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4347" s="1">
+        <v>45058</v>
+      </c>
+      <c r="B4347" s="21">
+        <v>5.1891579501595942E-4</v>
+      </c>
+      <c r="C4347" s="23">
+        <v>2.1708348835539054E-6</v>
+      </c>
+      <c r="D4347" s="21">
+        <v>5.2082644964242665E-4</v>
+      </c>
+    </row>
+    <row r="4348" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4348" s="1">
+        <v>45061</v>
+      </c>
+      <c r="B4348" s="21">
+        <v>-1.0872425746912813E-3</v>
+      </c>
+      <c r="C4348" s="23">
+        <v>1.9546570932210406E-4</v>
+      </c>
+      <c r="D4348" s="21">
+        <v>-8.9210542322912549E-4</v>
+      </c>
+    </row>
+    <row r="4349" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4349" s="1">
+        <v>45062</v>
+      </c>
+      <c r="B4349" s="21">
+        <v>2.2730821396942324E-3</v>
+      </c>
+      <c r="C4349" s="23">
+        <v>-3.7836258546431011E-5</v>
+      </c>
+      <c r="D4349" s="21">
+        <v>2.2338200382614119E-3</v>
+      </c>
+    </row>
+    <row r="4350" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4350" s="1">
+        <v>45063</v>
+      </c>
+      <c r="B4350" s="21">
+        <v>-4.0916531879393644E-3</v>
+      </c>
+      <c r="C4350" s="23">
+        <v>1.4241559728445062E-4</v>
+      </c>
+      <c r="D4350" s="21">
+        <v>-3.9473986198388109E-3</v>
+      </c>
+    </row>
+    <row r="4351" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4351" s="1">
+        <v>45064</v>
+      </c>
+      <c r="B4351" s="21">
+        <v>-3.3874881145017281E-3</v>
+      </c>
+      <c r="C4351" s="23">
+        <v>4.9335460763593418E-5</v>
+      </c>
+      <c r="D4351" s="21">
+        <v>-3.3355568015115493E-3</v>
+      </c>
+    </row>
+    <row r="4352" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4352" s="1">
+        <v>45065</v>
+      </c>
+      <c r="B4352" s="21">
+        <v>5.6814897881550389E-4</v>
+      </c>
+      <c r="C4352" s="23">
+        <v>5.0269828638372833E-5</v>
+      </c>
+      <c r="D4352" s="21">
+        <v>6.1803753724523213E-4</v>
+      </c>
+    </row>
+    <row r="4353" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4353" s="1">
+        <v>45068</v>
+      </c>
+      <c r="B4353" s="21">
+        <v>-2.0419230684110664E-5</v>
+      </c>
+      <c r="C4353" s="23">
+        <v>5.3341698094712682E-5</v>
+      </c>
+      <c r="D4353" s="21">
+        <v>3.3012126977018833E-5</v>
+      </c>
+    </row>
+    <row r="4354" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4354" s="1">
+        <v>45069</v>
+      </c>
+      <c r="B4354" s="21">
+        <v>3.417623366784331E-3</v>
+      </c>
+      <c r="C4354" s="23">
+        <v>-1.6318318484106365E-5</v>
+      </c>
+      <c r="D4354" s="21">
+        <v>3.3980594860832914E-3</v>
+      </c>
+    </row>
+    <row r="4355" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4355" s="1">
+        <v>45070</v>
+      </c>
+      <c r="B4355" s="21">
+        <v>2.4974439683574929E-3</v>
+      </c>
+      <c r="C4355" s="23">
+        <v>-9.6970698786515998E-5</v>
+      </c>
+      <c r="D4355" s="21">
+        <v>2.3983649168500768E-3</v>
+      </c>
+    </row>
+    <row r="4356" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4356" s="1">
+        <v>45071</v>
+      </c>
+      <c r="B4356" s="21">
+        <v>-2.5791355523288656E-3</v>
+      </c>
+      <c r="C4356" s="23">
+        <v>5.9652673496933988E-5</v>
+      </c>
+      <c r="D4356" s="21">
+        <v>-2.5176255699742001E-3</v>
+      </c>
+    </row>
+    <row r="4357" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4357" s="1">
+        <v>45072</v>
+      </c>
+      <c r="B4357" s="21">
+        <v>-4.0233302918201517E-3</v>
+      </c>
+      <c r="C4357" s="23">
+        <v>3.4050009397492131E-5</v>
+      </c>
+      <c r="D4357" s="21">
+        <v>-3.9857801338356756E-3</v>
+      </c>
+    </row>
+    <row r="4358" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4358" s="1">
+        <v>45076</v>
+      </c>
+      <c r="B4358" s="21">
+        <v>-1.0784882997580781E-4</v>
+      </c>
+      <c r="C4358" s="23">
+        <v>1.1273789378294004E-4</v>
+      </c>
+      <c r="D4358" s="21">
+        <v>5.2219904781006814E-6</v>
+      </c>
+    </row>
+    <row r="4359" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4359" s="1">
+        <v>45077</v>
+      </c>
+      <c r="B4359" s="21">
+        <v>0</v>
+      </c>
+      <c r="C4359" s="23">
+        <v>0</v>
+      </c>
+      <c r="D4359" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4360" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4360" s="1">
+        <v>45078</v>
+      </c>
+      <c r="B4360" s="24">
+        <v>-3.4529248451430701E-3</v>
+      </c>
+      <c r="C4360" s="25">
+        <v>1.6531641278126918E-3</v>
+      </c>
+      <c r="D4360" s="24">
+        <v>-1.7997607173303783E-3</v>
+      </c>
+    </row>
+    <row r="4361" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4361" s="1">
+        <v>45079</v>
+      </c>
+      <c r="B4361" s="24">
+        <v>-5.5515811331628556E-3</v>
+      </c>
+      <c r="C4361" s="25">
+        <v>1.1120547396191677E-3</v>
+      </c>
+      <c r="D4361" s="24">
+        <v>-4.4264854066662128E-3</v>
+      </c>
+    </row>
+    <row r="4362" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4362" s="1">
+        <v>45082</v>
+      </c>
+      <c r="B4362" s="24">
+        <v>6.355283425254801E-4</v>
+      </c>
+      <c r="C4362" s="25">
+        <v>1.8579621976923336E-4</v>
+      </c>
+      <c r="D4362" s="24">
+        <v>8.2123490305208635E-4</v>
+      </c>
+    </row>
+    <row r="4363" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4363" s="1">
+        <v>45083</v>
+      </c>
+      <c r="B4363" s="24">
+        <v>-8.0912118350120793E-4</v>
+      </c>
+      <c r="C4363" s="25">
+        <v>6.4110459667188191E-4</v>
+      </c>
+      <c r="D4363" s="24">
+        <v>-1.6022811849205137E-4</v>
+      </c>
+    </row>
+    <row r="4364" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4364" s="1">
+        <v>45084</v>
+      </c>
+      <c r="B4364" s="24">
+        <v>1.406382588319161E-3</v>
+      </c>
+      <c r="C4364" s="25">
+        <v>-1.3151181150354875E-4</v>
+      </c>
+      <c r="D4364" s="24">
+        <v>1.2685735192283303E-3</v>
+      </c>
+    </row>
+    <row r="4365" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4365" s="1">
+        <v>45085</v>
+      </c>
+      <c r="B4365" s="24">
+        <v>-2.1813051732923958E-3</v>
+      </c>
+      <c r="C4365" s="25">
+        <v>3.7996341225218354E-4</v>
+      </c>
+      <c r="D4365" s="24">
+        <v>-1.7907893348757253E-3</v>
+      </c>
+    </row>
+    <row r="4366" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4366" s="1">
+        <v>45086</v>
+      </c>
+      <c r="B4366" s="24">
+        <v>-6.2528821836801854E-4</v>
+      </c>
+      <c r="C4366" s="25">
+        <v>1.9686639474369624E-5</v>
+      </c>
+      <c r="D4366" s="24">
+        <v>-6.0298555551788571E-4</v>
+      </c>
+    </row>
+    <row r="4367" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4367" s="1">
+        <v>45089</v>
+      </c>
+      <c r="B4367" s="24">
+        <v>-3.4444006813017891E-3</v>
+      </c>
+      <c r="C4367" s="25">
+        <v>2.1430285746588455E-4</v>
+      </c>
+      <c r="D4367" s="24">
+        <v>-3.214418554221866E-3</v>
+      </c>
+    </row>
+    <row r="4368" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4368" s="1">
+        <v>45090</v>
+      </c>
+      <c r="B4368" s="24">
+        <v>-2.5626368979258206E-3</v>
+      </c>
+      <c r="C4368" s="25">
+        <v>2.4407863675597876E-4</v>
+      </c>
+      <c r="D4368" s="24">
+        <v>-2.30455667632829E-3</v>
+      </c>
+    </row>
+    <row r="4369" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4369" s="1">
+        <v>45091</v>
+      </c>
+      <c r="B4369" s="24">
+        <v>-1.5712162213886934E-4</v>
+      </c>
+      <c r="C4369" s="25">
+        <v>2.9686594538194194E-4</v>
+      </c>
+      <c r="D4369" s="24">
+        <v>1.4538572881294675E-4</v>
+      </c>
+    </row>
+    <row r="4370" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4370" s="1">
+        <v>45092</v>
+      </c>
+      <c r="B4370" s="24">
+        <v>-4.676011664833341E-3</v>
+      </c>
+      <c r="C4370" s="25">
+        <v>8.4291812026697616E-5</v>
+      </c>
+      <c r="D4370" s="24">
+        <v>-4.5684166675036501E-3</v>
+      </c>
+    </row>
+    <row r="4371" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4371" s="1">
+        <v>45093</v>
+      </c>
+      <c r="B4371" s="24">
+        <v>1.6127447620554694E-3</v>
+      </c>
+      <c r="C4371" s="25">
+        <v>2.6130266089780538E-4</v>
+      </c>
+      <c r="D4371" s="24">
+        <v>1.8719684147573044E-3</v>
+      </c>
+    </row>
+    <row r="4372" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4372" s="1">
+        <v>45097</v>
+      </c>
+      <c r="B4372" s="24">
+        <v>1.6824283140494331E-3</v>
+      </c>
+      <c r="C4372" s="25">
+        <v>-1.0684086546004713E-4</v>
+      </c>
+      <c r="D4372" s="24">
+        <v>1.5649679779407588E-3</v>
+      </c>
+    </row>
+    <row r="4373" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4373" s="1">
+        <v>45098</v>
+      </c>
+      <c r="B4373" s="24">
+        <v>2.3256071930419747E-3</v>
+      </c>
+      <c r="C4373" s="25">
+        <v>1.2527339051596081E-4</v>
+      </c>
+      <c r="D4373" s="24">
+        <v>2.4417049868759363E-3</v>
+      </c>
+    </row>
+    <row r="4374" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4374" s="1">
+        <v>45099</v>
+      </c>
+      <c r="B4374" s="24">
+        <v>-1.2907552620005003E-3</v>
+      </c>
+      <c r="C4374" s="25">
+        <v>2.9147142430891343E-4</v>
+      </c>
+      <c r="D4374" s="24">
+        <v>-9.8814091916263813E-4</v>
+      </c>
+    </row>
+    <row r="4375" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4375" s="1">
+        <v>45100</v>
+      </c>
+      <c r="B4375" s="24">
+        <v>3.1253553651964978E-3</v>
+      </c>
+      <c r="C4375" s="25">
+        <v>-2.7412922053453732E-4</v>
+      </c>
+      <c r="D4375" s="24">
+        <v>2.8298071564375935E-3</v>
+      </c>
+    </row>
+    <row r="4376" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4376" s="1">
+        <v>45103</v>
+      </c>
+      <c r="B4376" s="24">
+        <v>1.6886766175825932E-3</v>
+      </c>
+      <c r="C4376" s="25">
+        <v>-1.6448108932226069E-5</v>
+      </c>
+      <c r="D4376" s="24">
+        <v>1.6634664443736765E-3</v>
+      </c>
+    </row>
+    <row r="4377" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4377" s="1">
+        <v>45104</v>
+      </c>
+      <c r="B4377" s="24">
+        <v>-4.2584445580055421E-3</v>
+      </c>
+      <c r="C4377" s="25">
+        <v>4.2168201672155854E-4</v>
+      </c>
+      <c r="D4377" s="24">
+        <v>-3.8101495945725926E-3</v>
+      </c>
+    </row>
+    <row r="4378" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4378" s="1">
+        <v>45105</v>
+      </c>
+      <c r="B4378" s="24">
+        <v>1.1162211639184837E-4</v>
+      </c>
+      <c r="C4378" s="25">
+        <v>2.3743048818866501E-4</v>
+      </c>
+      <c r="D4378" s="24">
+        <v>3.5239406382956058E-4</v>
+      </c>
+    </row>
+    <row r="4379" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4379" s="1">
+        <v>45106</v>
+      </c>
+      <c r="B4379" s="24">
+        <v>-1.5606035244983714E-3</v>
+      </c>
+      <c r="C4379" s="25">
+        <v>3.2228635552411287E-5</v>
+      </c>
+      <c r="D4379" s="24">
+        <v>-1.5189249011999034E-3</v>
+      </c>
+    </row>
+    <row r="4380" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4380" s="1">
+        <v>45107</v>
+      </c>
+      <c r="B4380" s="24">
+        <v>-4.6124553687082173E-3</v>
+      </c>
+      <c r="C4380" s="25">
+        <v>1.165372752103655E-4</v>
+      </c>
+      <c r="D4380" s="24">
+        <v>-4.4672608059229818E-3</v>
+      </c>
+    </row>
+    <row r="4381" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4381" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Data and other scripts
</commit_message>
<xml_diff>
--- a/EquityHedging/data/update_strats/put_spread_data.xlsx
+++ b/EquityHedging/data/update_strats/put_spread_data.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\AC_MNG\Accounts\UPS\Presentations\2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nisa.local\nisa\Client\AC_MNG\Accounts\UPS\Presentations\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D62448E-692F-4CCD-B4D9-099AE5C8BA65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193C3692-51FF-4763-9BAD-C3DFBF900CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
     <t>Source: Bloomberg, NISA Calculations</t>
   </si>
   <si>
-    <t>As of March 31, 2023</t>
+    <t>As of August 31, 2023</t>
   </si>
 </sst>
 </file>
@@ -178,7 +178,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -233,6 +233,12 @@
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1014,7 +1020,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC4C8DD6-FF5C-406D-BA83-C4AD34B704D1}">
-  <sheetPr>
+  <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B9:B25"/>
@@ -1079,7 +1085,8 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D210"/>
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:D215"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A184" activePane="bottomLeft" state="frozen"/>
@@ -4024,6 +4031,76 @@
         <v>-4.860041175942742E-3</v>
       </c>
     </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A211" s="8">
+        <v>45044</v>
+      </c>
+      <c r="B211" s="7">
+        <v>-4.8623083254185628E-3</v>
+      </c>
+      <c r="C211" s="7">
+        <v>4.1621772599536033E-3</v>
+      </c>
+      <c r="D211" s="7">
+        <v>-7.0013106546495951E-4</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A212" s="8">
+        <v>45077</v>
+      </c>
+      <c r="B212" s="7">
+        <v>-2.1742339346643158E-3</v>
+      </c>
+      <c r="C212" s="7">
+        <v>1.0359947984193152E-3</v>
+      </c>
+      <c r="D212" s="7">
+        <v>-1.1382391362454447E-3</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A213" s="8">
+        <v>45107</v>
+      </c>
+      <c r="B213" s="7">
+        <v>-2.2418475489018541E-2</v>
+      </c>
+      <c r="C213" s="7">
+        <v>5.8024350296412841E-3</v>
+      </c>
+      <c r="D213" s="7">
+        <v>-1.6616040459376813E-2</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A214" s="8">
+        <v>45138</v>
+      </c>
+      <c r="B214" s="7">
+        <v>-1.0863494642860294E-2</v>
+      </c>
+      <c r="C214" s="7">
+        <v>1.0271451123518016E-3</v>
+      </c>
+      <c r="D214" s="7">
+        <v>-9.8363495305087145E-3</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A215" s="8">
+        <v>45169</v>
+      </c>
+      <c r="B215" s="7">
+        <v>1.6808372347838496E-3</v>
+      </c>
+      <c r="C215" s="7">
+        <v>3.6605933997102547E-4</v>
+      </c>
+      <c r="D215" s="7">
+        <v>2.046896574754431E-3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4031,10 +4108,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F4318"/>
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:F4423"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A4279" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A4392" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -64487,6 +64565,1476 @@
         <v>-4.5892271003205335E-3</v>
       </c>
     </row>
+    <row r="4319" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4319" s="1">
+        <v>45019</v>
+      </c>
+      <c r="B4319" s="21">
+        <v>-1.6120511520563189E-3</v>
+      </c>
+      <c r="C4319" s="23">
+        <v>7.9288211264479797E-4</v>
+      </c>
+      <c r="D4319" s="21">
+        <v>-8.1916903941152094E-4</v>
+      </c>
+    </row>
+    <row r="4320" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4320" s="1">
+        <v>45020</v>
+      </c>
+      <c r="B4320" s="21">
+        <v>2.4866218466028439E-3</v>
+      </c>
+      <c r="C4320" s="23">
+        <v>-3.2766895154749367E-4</v>
+      </c>
+      <c r="D4320" s="21">
+        <v>2.1564510285098171E-3</v>
+      </c>
+    </row>
+    <row r="4321" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4321" s="1">
+        <v>45021</v>
+      </c>
+      <c r="B4321" s="21">
+        <v>1.167090347724565E-3</v>
+      </c>
+      <c r="C4321" s="23">
+        <v>-2.4499279904672785E-4</v>
+      </c>
+      <c r="D4321" s="21">
+        <v>9.217686268351928E-4</v>
+      </c>
+    </row>
+    <row r="4322" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4322" s="1">
+        <v>45022</v>
+      </c>
+      <c r="B4322" s="21">
+        <v>-1.4991599634445103E-3</v>
+      </c>
+      <c r="C4322" s="23">
+        <v>7.7284077970457814E-4</v>
+      </c>
+      <c r="D4322" s="21">
+        <v>-7.2756235687753128E-4</v>
+      </c>
+    </row>
+    <row r="4323" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4323" s="1">
+        <v>45026</v>
+      </c>
+      <c r="B4323" s="21">
+        <v>-4.2810349389961114E-4</v>
+      </c>
+      <c r="C4323" s="23">
+        <v>4.4519113069776744E-4</v>
+      </c>
+      <c r="D4323" s="21">
+        <v>1.7273574351700174E-5</v>
+      </c>
+    </row>
+    <row r="4324" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4324" s="1">
+        <v>45027</v>
+      </c>
+      <c r="B4324" s="21">
+        <v>-2.4724651683640841E-5</v>
+      </c>
+      <c r="C4324" s="23">
+        <v>6.4698239718435894E-5</v>
+      </c>
+      <c r="D4324" s="21">
+        <v>4.0002114975257851E-5</v>
+      </c>
+    </row>
+    <row r="4325" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4325" s="1">
+        <v>45028</v>
+      </c>
+      <c r="B4325" s="21">
+        <v>1.7326335049369208E-3</v>
+      </c>
+      <c r="C4325" s="23">
+        <v>-1.9982519756397556E-4</v>
+      </c>
+      <c r="D4325" s="21">
+        <v>1.5302244345263313E-3</v>
+      </c>
+    </row>
+    <row r="4326" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4326" s="1">
+        <v>45029</v>
+      </c>
+      <c r="B4326" s="21">
+        <v>-5.3714924748913652E-3</v>
+      </c>
+      <c r="C4326" s="23">
+        <v>1.1655208250702872E-3</v>
+      </c>
+      <c r="D4326" s="21">
+        <v>-4.2011037244666866E-3</v>
+      </c>
+    </row>
+    <row r="4327" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4327" s="1">
+        <v>45030</v>
+      </c>
+      <c r="B4327" s="21">
+        <v>8.9999287825092106E-4</v>
+      </c>
+      <c r="C4327" s="23">
+        <v>3.5094170836805216E-4</v>
+      </c>
+      <c r="D4327" s="21">
+        <v>1.2499614971569432E-3</v>
+      </c>
+    </row>
+    <row r="4328" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4328" s="1">
+        <v>45033</v>
+      </c>
+      <c r="B4328" s="21">
+        <v>-1.2302428757698118E-3</v>
+      </c>
+      <c r="C4328" s="23">
+        <v>2.5597072766960627E-4</v>
+      </c>
+      <c r="D4328" s="21">
+        <v>-9.7011803059300324E-4</v>
+      </c>
+    </row>
+    <row r="4329" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4329" s="1">
+        <v>45034</v>
+      </c>
+      <c r="B4329" s="21">
+        <v>-3.1449510538695896E-4</v>
+      </c>
+      <c r="C4329" s="23">
+        <v>2.5086083487847552E-5</v>
+      </c>
+      <c r="D4329" s="21">
+        <v>-2.8834219879487051E-4</v>
+      </c>
+    </row>
+    <row r="4330" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4330" s="1">
+        <v>45035</v>
+      </c>
+      <c r="B4330" s="21">
+        <v>1.4510385912955821E-4</v>
+      </c>
+      <c r="C4330" s="23">
+        <v>2.1576046728886163E-5</v>
+      </c>
+      <c r="D4330" s="21">
+        <v>1.6631992932990381E-4</v>
+      </c>
+    </row>
+    <row r="4331" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4331" s="1">
+        <v>45036</v>
+      </c>
+      <c r="B4331" s="21">
+        <v>2.559688048210875E-3</v>
+      </c>
+      <c r="C4331" s="23">
+        <v>-3.3233151383815264E-4</v>
+      </c>
+      <c r="D4331" s="21">
+        <v>2.2179968295085958E-3</v>
+      </c>
+    </row>
+    <row r="4332" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4332" s="1">
+        <v>45037</v>
+      </c>
+      <c r="B4332" s="21">
+        <v>-4.1180719427366355E-4</v>
+      </c>
+      <c r="C4332" s="23">
+        <v>2.747543874344987E-4</v>
+      </c>
+      <c r="D4332" s="21">
+        <v>-1.3548880094220222E-4</v>
+      </c>
+    </row>
+    <row r="4333" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4333" s="1">
+        <v>45040</v>
+      </c>
+      <c r="B4333" s="21">
+        <v>-2.689260458037956E-4</v>
+      </c>
+      <c r="C4333" s="23">
+        <v>2.7500195085731132E-4</v>
+      </c>
+      <c r="D4333" s="21">
+        <v>7.4289668550769488E-6</v>
+      </c>
+    </row>
+    <row r="4334" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4334" s="1">
+        <v>45041</v>
+      </c>
+      <c r="B4334" s="21">
+        <v>6.4215417809489151E-3</v>
+      </c>
+      <c r="C4334" s="23">
+        <v>-7.4450882130068779E-4</v>
+      </c>
+      <c r="D4334" s="21">
+        <v>5.6539553463439652E-3</v>
+      </c>
+    </row>
+    <row r="4335" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4335" s="1">
+        <v>45042</v>
+      </c>
+      <c r="B4335" s="21">
+        <v>1.63233083957748E-3</v>
+      </c>
+      <c r="C4335" s="23">
+        <v>-8.1510862656810732E-6</v>
+      </c>
+      <c r="D4335" s="21">
+        <v>1.6200041774286828E-3</v>
+      </c>
+    </row>
+    <row r="4336" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4336" s="1">
+        <v>45043</v>
+      </c>
+      <c r="B4336" s="21">
+        <v>-7.3869270510031476E-3</v>
+      </c>
+      <c r="C4336" s="23">
+        <v>1.1327191911226977E-3</v>
+      </c>
+      <c r="D4336" s="21">
+        <v>-6.241821636621841E-3</v>
+      </c>
+    </row>
+    <row r="4337" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4337" s="1">
+        <v>45044</v>
+      </c>
+      <c r="B4337" s="21">
+        <v>-3.2896627872953184E-3</v>
+      </c>
+      <c r="C4337" s="23">
+        <v>4.3657000589871717E-4</v>
+      </c>
+      <c r="D4337" s="21">
+        <v>-2.8401810127393181E-3</v>
+      </c>
+    </row>
+    <row r="4338" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4338" s="1">
+        <v>45047</v>
+      </c>
+      <c r="B4338" s="21">
+        <v>2.553960562255486E-4</v>
+      </c>
+      <c r="C4338" s="23">
+        <v>-1.926689803120085E-5</v>
+      </c>
+      <c r="D4338" s="21">
+        <v>2.3612915819434775E-4</v>
+      </c>
+    </row>
+    <row r="4339" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4339" s="1">
+        <v>45048</v>
+      </c>
+      <c r="B4339" s="21">
+        <v>4.7486348650108475E-3</v>
+      </c>
+      <c r="C4339" s="23">
+        <v>-4.2016628799237694E-4</v>
+      </c>
+      <c r="D4339" s="21">
+        <v>4.3286673303636544E-3</v>
+      </c>
+    </row>
+    <row r="4340" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4340" s="1">
+        <v>45049</v>
+      </c>
+      <c r="B4340" s="21">
+        <v>2.8573037015260927E-3</v>
+      </c>
+      <c r="C4340" s="23">
+        <v>-8.8025255438341172E-5</v>
+      </c>
+      <c r="D4340" s="21">
+        <v>2.7709668957267893E-3</v>
+      </c>
+    </row>
+    <row r="4341" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4341" s="1">
+        <v>45050</v>
+      </c>
+      <c r="B4341" s="21">
+        <v>2.9495077265187541E-3</v>
+      </c>
+      <c r="C4341" s="23">
+        <v>-6.871228184305877E-4</v>
+      </c>
+      <c r="D4341" s="21">
+        <v>2.2693020384765461E-3</v>
+      </c>
+    </row>
+    <row r="4342" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4342" s="1">
+        <v>45051</v>
+      </c>
+      <c r="B4342" s="21">
+        <v>-7.4539082677605251E-3</v>
+      </c>
+      <c r="C4342" s="23">
+        <v>1.3029968734906954E-3</v>
+      </c>
+      <c r="D4342" s="21">
+        <v>-6.1738774155756281E-3</v>
+      </c>
+    </row>
+    <row r="4343" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4343" s="1">
+        <v>45054</v>
+      </c>
+      <c r="B4343" s="21">
+        <v>-2.3606074715439818E-4</v>
+      </c>
+      <c r="C4343" s="23">
+        <v>2.5226518509636857E-4</v>
+      </c>
+      <c r="D4343" s="21">
+        <v>1.5391586892434871E-5</v>
+      </c>
+    </row>
+    <row r="4344" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4344" s="1">
+        <v>45055</v>
+      </c>
+      <c r="B4344" s="21">
+        <v>1.729260295182096E-3</v>
+      </c>
+      <c r="C4344" s="23">
+        <v>-5.0831198038318202E-5</v>
+      </c>
+      <c r="D4344" s="21">
+        <v>1.6779998850744847E-3</v>
+      </c>
+    </row>
+    <row r="4345" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4345" s="1">
+        <v>45056</v>
+      </c>
+      <c r="B4345" s="21">
+        <v>-1.6476612254815134E-3</v>
+      </c>
+      <c r="C4345" s="23">
+        <v>1.6042739948666777E-4</v>
+      </c>
+      <c r="D4345" s="21">
+        <v>-1.487528737058633E-3</v>
+      </c>
+    </row>
+    <row r="4346" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4346" s="1">
+        <v>45057</v>
+      </c>
+      <c r="B4346" s="21">
+        <v>7.3158891907633102E-4</v>
+      </c>
+      <c r="C4346" s="23">
+        <v>3.813790210104407E-5</v>
+      </c>
+      <c r="D4346" s="21">
+        <v>7.6927943777817796E-4</v>
+      </c>
+    </row>
+    <row r="4347" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4347" s="1">
+        <v>45058</v>
+      </c>
+      <c r="B4347" s="21">
+        <v>5.1891579501595942E-4</v>
+      </c>
+      <c r="C4347" s="23">
+        <v>2.1708348835539054E-6</v>
+      </c>
+      <c r="D4347" s="21">
+        <v>5.2082644964242665E-4</v>
+      </c>
+    </row>
+    <row r="4348" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4348" s="1">
+        <v>45061</v>
+      </c>
+      <c r="B4348" s="21">
+        <v>-1.0872425746912813E-3</v>
+      </c>
+      <c r="C4348" s="23">
+        <v>1.9546570932210406E-4</v>
+      </c>
+      <c r="D4348" s="21">
+        <v>-8.9210542322912549E-4</v>
+      </c>
+    </row>
+    <row r="4349" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4349" s="1">
+        <v>45062</v>
+      </c>
+      <c r="B4349" s="21">
+        <v>2.2730821396942324E-3</v>
+      </c>
+      <c r="C4349" s="23">
+        <v>-3.7836258546431011E-5</v>
+      </c>
+      <c r="D4349" s="21">
+        <v>2.2338200382614119E-3</v>
+      </c>
+    </row>
+    <row r="4350" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4350" s="1">
+        <v>45063</v>
+      </c>
+      <c r="B4350" s="21">
+        <v>-4.0916531879393644E-3</v>
+      </c>
+      <c r="C4350" s="23">
+        <v>1.4241559728445062E-4</v>
+      </c>
+      <c r="D4350" s="21">
+        <v>-3.9473986198388109E-3</v>
+      </c>
+    </row>
+    <row r="4351" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4351" s="1">
+        <v>45064</v>
+      </c>
+      <c r="B4351" s="21">
+        <v>-3.3874881145017281E-3</v>
+      </c>
+      <c r="C4351" s="23">
+        <v>4.9335460763593418E-5</v>
+      </c>
+      <c r="D4351" s="21">
+        <v>-3.3355568015115493E-3</v>
+      </c>
+    </row>
+    <row r="4352" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4352" s="1">
+        <v>45065</v>
+      </c>
+      <c r="B4352" s="21">
+        <v>5.6814897881550389E-4</v>
+      </c>
+      <c r="C4352" s="23">
+        <v>5.0269828638372833E-5</v>
+      </c>
+      <c r="D4352" s="21">
+        <v>6.1803753724523213E-4</v>
+      </c>
+    </row>
+    <row r="4353" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4353" s="1">
+        <v>45068</v>
+      </c>
+      <c r="B4353" s="21">
+        <v>-2.0419230684110664E-5</v>
+      </c>
+      <c r="C4353" s="23">
+        <v>5.3341698094712682E-5</v>
+      </c>
+      <c r="D4353" s="21">
+        <v>3.3012126977018833E-5</v>
+      </c>
+    </row>
+    <row r="4354" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4354" s="1">
+        <v>45069</v>
+      </c>
+      <c r="B4354" s="21">
+        <v>3.417623366784331E-3</v>
+      </c>
+      <c r="C4354" s="23">
+        <v>-1.6318318484106365E-5</v>
+      </c>
+      <c r="D4354" s="21">
+        <v>3.3980594860832914E-3</v>
+      </c>
+    </row>
+    <row r="4355" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4355" s="1">
+        <v>45070</v>
+      </c>
+      <c r="B4355" s="21">
+        <v>2.4974439683574929E-3</v>
+      </c>
+      <c r="C4355" s="23">
+        <v>-9.6970698786515998E-5</v>
+      </c>
+      <c r="D4355" s="21">
+        <v>2.3983649168500768E-3</v>
+      </c>
+    </row>
+    <row r="4356" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4356" s="1">
+        <v>45071</v>
+      </c>
+      <c r="B4356" s="21">
+        <v>-2.5791355523288656E-3</v>
+      </c>
+      <c r="C4356" s="23">
+        <v>5.9652673496933988E-5</v>
+      </c>
+      <c r="D4356" s="21">
+        <v>-2.5176255699742001E-3</v>
+      </c>
+    </row>
+    <row r="4357" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4357" s="1">
+        <v>45072</v>
+      </c>
+      <c r="B4357" s="21">
+        <v>-4.0233302918201517E-3</v>
+      </c>
+      <c r="C4357" s="23">
+        <v>3.4050009397492131E-5</v>
+      </c>
+      <c r="D4357" s="21">
+        <v>-3.9857801338356756E-3</v>
+      </c>
+    </row>
+    <row r="4358" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4358" s="1">
+        <v>45076</v>
+      </c>
+      <c r="B4358" s="21">
+        <v>-1.0784882997580781E-4</v>
+      </c>
+      <c r="C4358" s="23">
+        <v>1.1273789378294004E-4</v>
+      </c>
+      <c r="D4358" s="21">
+        <v>5.2219904781006814E-6</v>
+      </c>
+    </row>
+    <row r="4359" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4359" s="1">
+        <v>45077</v>
+      </c>
+      <c r="B4359" s="21">
+        <v>0</v>
+      </c>
+      <c r="C4359" s="23">
+        <v>0</v>
+      </c>
+      <c r="D4359" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4360" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4360" s="1">
+        <v>45078</v>
+      </c>
+      <c r="B4360" s="24">
+        <v>-3.4529248451430701E-3</v>
+      </c>
+      <c r="C4360" s="25">
+        <v>1.6531641278126918E-3</v>
+      </c>
+      <c r="D4360" s="24">
+        <v>-1.7997607173303783E-3</v>
+      </c>
+    </row>
+    <row r="4361" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4361" s="1">
+        <v>45079</v>
+      </c>
+      <c r="B4361" s="24">
+        <v>-5.5515811331628556E-3</v>
+      </c>
+      <c r="C4361" s="25">
+        <v>1.1120547396191677E-3</v>
+      </c>
+      <c r="D4361" s="24">
+        <v>-4.4264854066662128E-3</v>
+      </c>
+    </row>
+    <row r="4362" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4362" s="1">
+        <v>45082</v>
+      </c>
+      <c r="B4362" s="24">
+        <v>6.355283425254801E-4</v>
+      </c>
+      <c r="C4362" s="25">
+        <v>1.8579621976923336E-4</v>
+      </c>
+      <c r="D4362" s="24">
+        <v>8.2123490305208635E-4</v>
+      </c>
+    </row>
+    <row r="4363" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4363" s="1">
+        <v>45083</v>
+      </c>
+      <c r="B4363" s="24">
+        <v>-8.0912118350120793E-4</v>
+      </c>
+      <c r="C4363" s="25">
+        <v>6.4110459667188191E-4</v>
+      </c>
+      <c r="D4363" s="24">
+        <v>-1.6022811849205137E-4</v>
+      </c>
+    </row>
+    <row r="4364" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4364" s="1">
+        <v>45084</v>
+      </c>
+      <c r="B4364" s="24">
+        <v>1.406382588319161E-3</v>
+      </c>
+      <c r="C4364" s="25">
+        <v>-1.3151181150354875E-4</v>
+      </c>
+      <c r="D4364" s="24">
+        <v>1.2685735192283303E-3</v>
+      </c>
+    </row>
+    <row r="4365" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4365" s="1">
+        <v>45085</v>
+      </c>
+      <c r="B4365" s="24">
+        <v>-2.1813051732923958E-3</v>
+      </c>
+      <c r="C4365" s="25">
+        <v>3.7996341225218354E-4</v>
+      </c>
+      <c r="D4365" s="24">
+        <v>-1.7907893348757253E-3</v>
+      </c>
+    </row>
+    <row r="4366" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4366" s="1">
+        <v>45086</v>
+      </c>
+      <c r="B4366" s="24">
+        <v>-6.2528821836801854E-4</v>
+      </c>
+      <c r="C4366" s="25">
+        <v>1.9686639474369624E-5</v>
+      </c>
+      <c r="D4366" s="24">
+        <v>-6.0298555551788571E-4</v>
+      </c>
+    </row>
+    <row r="4367" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4367" s="1">
+        <v>45089</v>
+      </c>
+      <c r="B4367" s="24">
+        <v>-3.4444006813017891E-3</v>
+      </c>
+      <c r="C4367" s="25">
+        <v>2.1430285746588455E-4</v>
+      </c>
+      <c r="D4367" s="24">
+        <v>-3.214418554221866E-3</v>
+      </c>
+    </row>
+    <row r="4368" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4368" s="1">
+        <v>45090</v>
+      </c>
+      <c r="B4368" s="24">
+        <v>-2.5626368979258206E-3</v>
+      </c>
+      <c r="C4368" s="25">
+        <v>2.4407863675597876E-4</v>
+      </c>
+      <c r="D4368" s="24">
+        <v>-2.30455667632829E-3</v>
+      </c>
+    </row>
+    <row r="4369" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4369" s="1">
+        <v>45091</v>
+      </c>
+      <c r="B4369" s="24">
+        <v>-1.5712162213886934E-4</v>
+      </c>
+      <c r="C4369" s="25">
+        <v>2.9686594538194194E-4</v>
+      </c>
+      <c r="D4369" s="24">
+        <v>1.4538572881294675E-4</v>
+      </c>
+    </row>
+    <row r="4370" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4370" s="1">
+        <v>45092</v>
+      </c>
+      <c r="B4370" s="24">
+        <v>-4.676011664833341E-3</v>
+      </c>
+      <c r="C4370" s="25">
+        <v>8.4291812026697616E-5</v>
+      </c>
+      <c r="D4370" s="24">
+        <v>-4.5684166675036501E-3</v>
+      </c>
+    </row>
+    <row r="4371" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4371" s="1">
+        <v>45093</v>
+      </c>
+      <c r="B4371" s="24">
+        <v>1.6127447620554694E-3</v>
+      </c>
+      <c r="C4371" s="25">
+        <v>2.6130266089780538E-4</v>
+      </c>
+      <c r="D4371" s="24">
+        <v>1.8719684147573044E-3</v>
+      </c>
+    </row>
+    <row r="4372" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4372" s="1">
+        <v>45097</v>
+      </c>
+      <c r="B4372" s="24">
+        <v>1.6824283140494331E-3</v>
+      </c>
+      <c r="C4372" s="25">
+        <v>-1.0684086546004713E-4</v>
+      </c>
+      <c r="D4372" s="24">
+        <v>1.5649679779407588E-3</v>
+      </c>
+    </row>
+    <row r="4373" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4373" s="1">
+        <v>45098</v>
+      </c>
+      <c r="B4373" s="24">
+        <v>2.3256071930419747E-3</v>
+      </c>
+      <c r="C4373" s="25">
+        <v>1.2527339051596081E-4</v>
+      </c>
+      <c r="D4373" s="24">
+        <v>2.4417049868759363E-3</v>
+      </c>
+    </row>
+    <row r="4374" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4374" s="1">
+        <v>45099</v>
+      </c>
+      <c r="B4374" s="24">
+        <v>-1.2907552620005003E-3</v>
+      </c>
+      <c r="C4374" s="25">
+        <v>2.9147142430891343E-4</v>
+      </c>
+      <c r="D4374" s="24">
+        <v>-9.8814091916263813E-4</v>
+      </c>
+    </row>
+    <row r="4375" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4375" s="1">
+        <v>45100</v>
+      </c>
+      <c r="B4375" s="24">
+        <v>3.1253553651964978E-3</v>
+      </c>
+      <c r="C4375" s="25">
+        <v>-2.7412922053453732E-4</v>
+      </c>
+      <c r="D4375" s="24">
+        <v>2.8298071564375935E-3</v>
+      </c>
+    </row>
+    <row r="4376" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4376" s="1">
+        <v>45103</v>
+      </c>
+      <c r="B4376" s="24">
+        <v>1.6886766175825932E-3</v>
+      </c>
+      <c r="C4376" s="25">
+        <v>-1.6448108932226069E-5</v>
+      </c>
+      <c r="D4376" s="24">
+        <v>1.6634664443736765E-3</v>
+      </c>
+    </row>
+    <row r="4377" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4377" s="1">
+        <v>45104</v>
+      </c>
+      <c r="B4377" s="24">
+        <v>-4.2584445580055421E-3</v>
+      </c>
+      <c r="C4377" s="25">
+        <v>4.2168201672155854E-4</v>
+      </c>
+      <c r="D4377" s="24">
+        <v>-3.8101495945725926E-3</v>
+      </c>
+    </row>
+    <row r="4378" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4378" s="1">
+        <v>45105</v>
+      </c>
+      <c r="B4378" s="24">
+        <v>1.1162211639184837E-4</v>
+      </c>
+      <c r="C4378" s="25">
+        <v>2.3743048818866501E-4</v>
+      </c>
+      <c r="D4378" s="24">
+        <v>3.5239406382956058E-4</v>
+      </c>
+    </row>
+    <row r="4379" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4379" s="1">
+        <v>45106</v>
+      </c>
+      <c r="B4379" s="24">
+        <v>-1.5606035244983714E-3</v>
+      </c>
+      <c r="C4379" s="25">
+        <v>3.2228635552411287E-5</v>
+      </c>
+      <c r="D4379" s="24">
+        <v>-1.5189249011999034E-3</v>
+      </c>
+    </row>
+    <row r="4380" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4380" s="1">
+        <v>45107</v>
+      </c>
+      <c r="B4380" s="24">
+        <v>-4.6124553687082173E-3</v>
+      </c>
+      <c r="C4380" s="25">
+        <v>1.165372752103655E-4</v>
+      </c>
+      <c r="D4380" s="24">
+        <v>-4.4672608059229818E-3</v>
+      </c>
+    </row>
+    <row r="4381" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4381" s="1">
+        <v>45110</v>
+      </c>
+      <c r="B4381" s="24">
+        <v>-3.5236758711522967E-4</v>
+      </c>
+      <c r="C4381" s="25">
+        <v>1.4245755685174559E-4</v>
+      </c>
+      <c r="D4381" s="24">
+        <v>-2.099100302634841E-4</v>
+      </c>
+    </row>
+    <row r="4382" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4382" s="1">
+        <v>45112</v>
+      </c>
+      <c r="B4382" s="24">
+        <v>7.3561416175339236E-4</v>
+      </c>
+      <c r="C4382" s="25">
+        <v>-2.8157666030814598E-5</v>
+      </c>
+      <c r="D4382" s="24">
+        <v>7.0734175599245061E-4</v>
+      </c>
+    </row>
+    <row r="4383" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4383" s="1">
+        <v>45113</v>
+      </c>
+      <c r="B4383" s="24">
+        <v>3.1927831412659783E-3</v>
+      </c>
+      <c r="C4383" s="25">
+        <v>-3.3063001612440742E-4</v>
+      </c>
+      <c r="D4383" s="24">
+        <v>2.861914948745038E-3</v>
+      </c>
+    </row>
+    <row r="4384" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4384" s="1">
+        <v>45114</v>
+      </c>
+      <c r="B4384" s="24">
+        <v>1.1444662698611976E-3</v>
+      </c>
+      <c r="C4384" s="25">
+        <v>1.1513243226467026E-4</v>
+      </c>
+      <c r="D4384" s="24">
+        <v>1.259435054515444E-3</v>
+      </c>
+    </row>
+    <row r="4385" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4385" s="1">
+        <v>45117</v>
+      </c>
+      <c r="B4385" s="24">
+        <v>-8.8436324935313904E-4</v>
+      </c>
+      <c r="C4385" s="25">
+        <v>1.4363559136050226E-4</v>
+      </c>
+      <c r="D4385" s="24">
+        <v>-7.4149243361384932E-4</v>
+      </c>
+    </row>
+    <row r="4386" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4386" s="1">
+        <v>45118</v>
+      </c>
+      <c r="B4386" s="24">
+        <v>-2.5365000714836208E-3</v>
+      </c>
+      <c r="C4386" s="25">
+        <v>1.2425579745217142E-4</v>
+      </c>
+      <c r="D4386" s="24">
+        <v>-2.41261218002409E-3</v>
+      </c>
+    </row>
+    <row r="4387" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4387" s="1">
+        <v>45119</v>
+      </c>
+      <c r="B4387" s="24">
+        <v>-2.9785321103148027E-3</v>
+      </c>
+      <c r="C4387" s="25">
+        <v>1.6410935218250875E-4</v>
+      </c>
+      <c r="D4387" s="24">
+        <v>-2.8141387247015348E-3</v>
+      </c>
+    </row>
+    <row r="4388" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4388" s="1">
+        <v>45120</v>
+      </c>
+      <c r="B4388" s="24">
+        <v>-3.1290397251605142E-3</v>
+      </c>
+      <c r="C4388" s="25">
+        <v>1.6408242472208307E-4</v>
+      </c>
+      <c r="D4388" s="24">
+        <v>-2.9636430066721405E-3</v>
+      </c>
+    </row>
+    <row r="4389" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4389" s="1">
+        <v>45121</v>
+      </c>
+      <c r="B4389" s="24">
+        <v>5.8211859549143076E-4</v>
+      </c>
+      <c r="C4389" s="25">
+        <v>7.109356087884328E-5</v>
+      </c>
+      <c r="D4389" s="24">
+        <v>6.5326664651204085E-4</v>
+      </c>
+    </row>
+    <row r="4390" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4390" s="1">
+        <v>45124</v>
+      </c>
+      <c r="B4390" s="24">
+        <v>-1.4529500174606589E-3</v>
+      </c>
+      <c r="C4390" s="25">
+        <v>9.0234808156123325E-5</v>
+      </c>
+      <c r="D4390" s="24">
+        <v>-1.3615061361463775E-3</v>
+      </c>
+    </row>
+    <row r="4391" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4391" s="1">
+        <v>45125</v>
+      </c>
+      <c r="B4391" s="24">
+        <v>-2.9554864532482373E-3</v>
+      </c>
+      <c r="C4391" s="25">
+        <v>6.3388182839551574E-5</v>
+      </c>
+      <c r="D4391" s="24">
+        <v>-2.8897867247751076E-3</v>
+      </c>
+    </row>
+    <row r="4392" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4392" s="1">
+        <v>45126</v>
+      </c>
+      <c r="B4392" s="24">
+        <v>-7.9204847211759638E-4</v>
+      </c>
+      <c r="C4392" s="25">
+        <v>-2.3702365544475251E-5</v>
+      </c>
+      <c r="D4392" s="24">
+        <v>-8.1538220975718094E-4</v>
+      </c>
+    </row>
+    <row r="4393" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4393" s="1">
+        <v>45127</v>
+      </c>
+      <c r="B4393" s="24">
+        <v>2.720587487301424E-3</v>
+      </c>
+      <c r="C4393" s="25">
+        <v>-5.3930677021521412E-5</v>
+      </c>
+      <c r="D4393" s="24">
+        <v>2.6642348288211143E-3</v>
+      </c>
+    </row>
+    <row r="4394" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4394" s="1">
+        <v>45128</v>
+      </c>
+      <c r="B4394" s="24">
+        <v>6.3840059461189037E-5</v>
+      </c>
+      <c r="C4394" s="25">
+        <v>5.38317009397074E-5</v>
+      </c>
+      <c r="D4394" s="24">
+        <v>1.1799403249782409E-4</v>
+      </c>
+    </row>
+    <row r="4395" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4395" s="1">
+        <v>45131</v>
+      </c>
+      <c r="B4395" s="24">
+        <v>-1.5910668692451435E-3</v>
+      </c>
+      <c r="C4395" s="25">
+        <v>9.5935285117461049E-5</v>
+      </c>
+      <c r="D4395" s="24">
+        <v>-1.4933760794420595E-3</v>
+      </c>
+    </row>
+    <row r="4396" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4396" s="1">
+        <v>45132</v>
+      </c>
+      <c r="B4396" s="24">
+        <v>-1.0436872092824789E-3</v>
+      </c>
+      <c r="C4396" s="25">
+        <v>5.3930217155821415E-5</v>
+      </c>
+      <c r="D4396" s="24">
+        <v>-9.884771795972613E-4</v>
+      </c>
+    </row>
+    <row r="4397" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4397" s="1">
+        <v>45133</v>
+      </c>
+      <c r="B4397" s="24">
+        <v>6.1244967173026114E-5</v>
+      </c>
+      <c r="C4397" s="25">
+        <v>7.3345059214748349E-5</v>
+      </c>
+      <c r="D4397" s="24">
+        <v>1.3522301090149175E-4</v>
+      </c>
+    </row>
+    <row r="4398" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4398" s="1">
+        <v>45134</v>
+      </c>
+      <c r="B4398" s="24">
+        <v>2.4988684645645982E-3</v>
+      </c>
+      <c r="C4398" s="25">
+        <v>-1.3108929605182027E-4</v>
+      </c>
+      <c r="D4398" s="24">
+        <v>2.3642462557014617E-3</v>
+      </c>
+    </row>
+    <row r="4399" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4399" s="1">
+        <v>45135</v>
+      </c>
+      <c r="B4399" s="24">
+        <v>-3.4987504399344848E-3</v>
+      </c>
+      <c r="C4399" s="25">
+        <v>1.8301858825774339E-4</v>
+      </c>
+      <c r="D4399" s="24">
+        <v>-3.3117194700176462E-3</v>
+      </c>
+    </row>
+    <row r="4400" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4400" s="1">
+        <v>45138</v>
+      </c>
+      <c r="B4400" s="24">
+        <v>-6.6772628244763516E-4</v>
+      </c>
+      <c r="C4400" s="25">
+        <v>5.5841655471604033E-5</v>
+      </c>
+      <c r="D4400" s="24">
+        <v>-6.1065501841299919E-4</v>
+      </c>
+    </row>
+    <row r="4401" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4401" s="1">
+        <v>45139</v>
+      </c>
+      <c r="B4401" s="24">
+        <v>1.1303389306608471E-4</v>
+      </c>
+      <c r="C4401" s="25">
+        <v>-8.6408981336244399E-6</v>
+      </c>
+      <c r="D4401" s="24">
+        <v>1.0439299493246028E-4</v>
+      </c>
+    </row>
+    <row r="4402" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4402" s="1">
+        <v>45140</v>
+      </c>
+      <c r="B4402" s="24">
+        <v>5.7565458464205882E-4</v>
+      </c>
+      <c r="C4402" s="25">
+        <v>-2.3359331376975978E-4</v>
+      </c>
+      <c r="D4402" s="24">
+        <v>3.4209264573125916E-4</v>
+      </c>
+    </row>
+    <row r="4403" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4403" s="1">
+        <v>45141</v>
+      </c>
+      <c r="B4403" s="24">
+        <v>2.345022387060873E-4</v>
+      </c>
+      <c r="C4403" s="25">
+        <v>1.308105254871341E-5</v>
+      </c>
+      <c r="D4403" s="24">
+        <v>2.476310642934383E-4</v>
+      </c>
+    </row>
+    <row r="4404" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4404" s="1">
+        <v>45142</v>
+      </c>
+      <c r="B4404" s="24">
+        <v>3.5639514209818513E-4</v>
+      </c>
+      <c r="C4404" s="25">
+        <v>-1.944066705562673E-4</v>
+      </c>
+      <c r="D4404" s="24">
+        <v>1.6224947829996062E-4</v>
+      </c>
+    </row>
+    <row r="4405" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4405" s="1">
+        <v>45145</v>
+      </c>
+      <c r="B4405" s="24">
+        <v>-7.4748119599391991E-4</v>
+      </c>
+      <c r="C4405" s="25">
+        <v>2.9927671330900991E-4</v>
+      </c>
+      <c r="D4405" s="24">
+        <v>-4.4890357095016248E-4</v>
+      </c>
+    </row>
+    <row r="4406" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4406" s="1">
+        <v>45146</v>
+      </c>
+      <c r="B4406" s="24">
+        <v>2.4302908131630923E-4</v>
+      </c>
+      <c r="C4406" s="25">
+        <v>5.0231121073017213E-5</v>
+      </c>
+      <c r="D4406" s="24">
+        <v>2.9326371756438848E-4</v>
+      </c>
+    </row>
+    <row r="4407" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4407" s="1">
+        <v>45147</v>
+      </c>
+      <c r="B4407" s="24">
+        <v>4.3918609927516751E-4</v>
+      </c>
+      <c r="C4407" s="25">
+        <v>4.3924296505382829E-5</v>
+      </c>
+      <c r="D4407" s="24">
+        <v>4.8310892351095678E-4</v>
+      </c>
+    </row>
+    <row r="4408" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4408" s="1">
+        <v>45148</v>
+      </c>
+      <c r="B4408" s="24">
+        <v>0</v>
+      </c>
+      <c r="C4408" s="25">
+        <v>2.5079854105909948E-5</v>
+      </c>
+      <c r="D4408" s="24">
+        <v>2.504943345084622E-5</v>
+      </c>
+    </row>
+    <row r="4409" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4409" s="1">
+        <v>45149</v>
+      </c>
+      <c r="B4409" s="24">
+        <v>6.958010302806894E-5</v>
+      </c>
+      <c r="C4409" s="25">
+        <v>1.3605545908219419E-4</v>
+      </c>
+      <c r="D4409" s="24">
+        <v>2.0547089483623121E-4</v>
+      </c>
+    </row>
+    <row r="4410" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4410" s="1">
+        <v>45152</v>
+      </c>
+      <c r="B4410" s="24">
+        <v>-2.7281067120319726E-4</v>
+      </c>
+      <c r="C4410" s="25">
+        <v>-2.0587148241910752E-6</v>
+      </c>
+      <c r="D4410" s="24">
+        <v>-2.7483108218139305E-4</v>
+      </c>
+    </row>
+    <row r="4411" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4411" s="1">
+        <v>45153</v>
+      </c>
+      <c r="B4411" s="24">
+        <v>5.5805487561800583E-4</v>
+      </c>
+      <c r="C4411" s="25">
+        <v>-1.0574985607609163E-5</v>
+      </c>
+      <c r="D4411" s="24">
+        <v>5.4741874208875875E-4</v>
+      </c>
+    </row>
+    <row r="4412" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4412" s="1">
+        <v>45154</v>
+      </c>
+      <c r="B4412" s="24">
+        <v>4.0796328124321574E-4</v>
+      </c>
+      <c r="C4412" s="25">
+        <v>4.6432607362094427E-5</v>
+      </c>
+      <c r="D4412" s="24">
+        <v>4.5427496315377669E-4</v>
+      </c>
+    </row>
+    <row r="4413" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4413" s="1">
+        <v>45155</v>
+      </c>
+      <c r="B4413" s="24">
+        <v>4.8530788509660796E-4</v>
+      </c>
+      <c r="C4413" s="25">
+        <v>-6.291327978458081E-5</v>
+      </c>
+      <c r="D4413" s="24">
+        <v>4.2243902179161179E-4</v>
+      </c>
+    </row>
+    <row r="4414" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4414" s="1">
+        <v>45156</v>
+      </c>
+      <c r="B4414" s="24">
+        <v>3.2675374515441325E-5</v>
+      </c>
+      <c r="C4414" s="25">
+        <v>2.5162017759698403E-5</v>
+      </c>
+      <c r="D4414" s="24">
+        <v>5.7772224570678854E-5</v>
+      </c>
+    </row>
+    <row r="4415" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4415" s="1">
+        <v>45159</v>
+      </c>
+      <c r="B4415" s="24">
+        <v>-4.5751531218677564E-4</v>
+      </c>
+      <c r="C4415" s="25">
+        <v>1.0406805621996893E-4</v>
+      </c>
+      <c r="D4415" s="24">
+        <v>-3.5364851538399728E-4</v>
+      </c>
+    </row>
+    <row r="4416" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4416" s="1">
+        <v>45160</v>
+      </c>
+      <c r="B4416" s="24">
+        <v>1.256182162944958E-4</v>
+      </c>
+      <c r="C4416" s="25">
+        <v>3.6476707705836575E-5</v>
+      </c>
+      <c r="D4416" s="24">
+        <v>1.6199177842218319E-4</v>
+      </c>
+    </row>
+    <row r="4417" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4417" s="1">
+        <v>45161</v>
+      </c>
+      <c r="B4417" s="24">
+        <v>-3.8511254373035974E-4</v>
+      </c>
+      <c r="C4417" s="25">
+        <v>2.5025774915767525E-5</v>
+      </c>
+      <c r="D4417" s="24">
+        <v>-3.6003802538439269E-4</v>
+      </c>
+    </row>
+    <row r="4418" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4418" s="1">
+        <v>45162</v>
+      </c>
+      <c r="B4418" s="24">
+        <v>2.3327177153951534E-4</v>
+      </c>
+      <c r="C4418" s="25">
+        <v>-1.9416084659538872E-5</v>
+      </c>
+      <c r="D4418" s="24">
+        <v>2.1382204126242313E-4</v>
+      </c>
+    </row>
+    <row r="4419" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4419" s="1">
+        <v>45163</v>
+      </c>
+      <c r="B4419" s="24">
+        <v>-1.6998246755056318E-4</v>
+      </c>
+      <c r="C4419" s="25">
+        <v>5.703165954504218E-5</v>
+      </c>
+      <c r="D4419" s="24">
+        <v>-1.1301897734201748E-4</v>
+      </c>
+    </row>
+    <row r="4420" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4420" s="1">
+        <v>45166</v>
+      </c>
+      <c r="B4420" s="24">
+        <v>-7.1408620470344704E-5</v>
+      </c>
+      <c r="C4420" s="25">
+        <v>1.6595511670787621E-5</v>
+      </c>
+      <c r="D4420" s="24">
+        <v>-5.4820080989223839E-5</v>
+      </c>
+    </row>
+    <row r="4421" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4421" s="1">
+        <v>45167</v>
+      </c>
+      <c r="B4421" s="24">
+        <v>-7.8575878673327795E-5</v>
+      </c>
+      <c r="C4421" s="25">
+        <v>9.6351571143890564E-6</v>
+      </c>
+      <c r="D4421" s="24">
+        <v>-6.8930550813169902E-5</v>
+      </c>
+    </row>
+    <row r="4422" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4422" s="1">
+        <v>45168</v>
+      </c>
+      <c r="B4422" s="24">
+        <v>-1.0660356071521539E-5</v>
+      </c>
+      <c r="C4422" s="25">
+        <v>9.6350642790309218E-6</v>
+      </c>
+      <c r="D4422" s="24">
+        <v>-1.0377645377751832E-6</v>
+      </c>
+    </row>
+    <row r="4423" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4423" s="1">
+        <v>45169</v>
+      </c>
+      <c r="B4423" s="24">
+        <v>0</v>
+      </c>
+      <c r="C4423" s="25">
+        <v>0</v>
+      </c>
+      <c r="D4423" s="24">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -64494,7 +66042,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7310C0A4-4698-4AEB-A328-CB88610FA53C}">
-  <sheetPr>
+  <sheetPr codeName="Sheet4">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1"/>

</xml_diff>